<commit_message>
Diagnostic Spreadsheet changes for Expanded Reproduction
</commit_message>
<xml_diff>
--- a/supplementary/Expanded Reproduction/spreadsheet illustrations (for Moscow Plekhanov).xlsx
+++ b/supplementary/Expanded Reproduction/spreadsheet illustrations (for Moscow Plekhanov).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\My Works\REPOS\simulation-api\supplementary\Expanded Reproduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E844D075-E9D5-420D-95CF-2C9388A71D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83310F19-F1AC-4EC2-BE3A-D95F3D29B1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="108">
   <si>
     <t>DI</t>
   </si>
@@ -525,6 +525,18 @@
   </si>
   <si>
     <t>Simulation start point</t>
+  </si>
+  <si>
+    <t>Consumption Goods</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Production period 1</t>
+  </si>
+  <si>
+    <t>Scale</t>
   </si>
 </sst>
 </file>
@@ -759,7 +771,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -875,6 +887,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1344,13 +1359,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>575734</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1397,13 +1412,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>55034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1450,13 +1465,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>529166</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>122767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1503,13 +1518,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>97367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>397933</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>122767</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1556,13 +1571,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>592666</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>55033</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>46567</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1606,13 +1621,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>67734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3193,43 +3208,51 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:AC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.61328125" customWidth="1"/>
-    <col min="5" max="7" width="8.921875" customWidth="1"/>
-    <col min="8" max="8" width="13.765625" customWidth="1"/>
-    <col min="11" max="11" width="10.3828125" customWidth="1"/>
-    <col min="12" max="13" width="12.84375" customWidth="1"/>
-    <col min="14" max="14" width="13.3046875" customWidth="1"/>
-    <col min="15" max="15" width="8.921875" style="3"/>
+    <col min="1" max="1" width="9.61328125" customWidth="1"/>
+    <col min="5" max="6" width="8.921875" customWidth="1"/>
+    <col min="7" max="7" width="7.61328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.07421875" customWidth="1"/>
+    <col min="10" max="10" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.53515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.765625" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.23046875" customWidth="1"/>
+    <col min="17" max="17" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.53515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.3046875" customWidth="1"/>
-    <col min="20" max="20" width="10.15234375" customWidth="1"/>
-    <col min="21" max="21" width="16.07421875" customWidth="1"/>
-    <col min="22" max="22" width="14.3828125" customWidth="1"/>
-    <col min="23" max="23" width="14.53515625" customWidth="1"/>
-    <col min="24" max="24" width="18.3046875" customWidth="1"/>
+    <col min="20" max="20" width="8.921875" style="3"/>
+    <col min="24" max="24" width="13.3046875" customWidth="1"/>
+    <col min="25" max="25" width="10.15234375" customWidth="1"/>
+    <col min="26" max="26" width="16.07421875" customWidth="1"/>
+    <col min="27" max="27" width="14.3828125" customWidth="1"/>
+    <col min="28" max="28" width="14.53515625" customWidth="1"/>
+    <col min="29" max="29" width="18.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="7">
         <v>0.1</v>
       </c>
-      <c r="O1"/>
-      <c r="Q1" s="65" t="s">
+      <c r="T1"/>
+      <c r="V1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="65"/>
-    </row>
-    <row r="2" spans="1:24" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="W1" s="65"/>
+    </row>
+    <row r="2" spans="1:29" ht="83.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -3242,151 +3265,216 @@
       <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="R2" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="X2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="Y2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6" t="s">
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="C4" s="6">
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>4000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="F4">
+        <v>4000</v>
+      </c>
+      <c r="G4">
+        <v>6000</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4">
+        <v>1500</v>
+      </c>
+      <c r="O4">
+        <v>250</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C5">
+        <v>1500</v>
+      </c>
+      <c r="D5">
+        <v>750</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>9500</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5">
+        <v>750</v>
+      </c>
+      <c r="O5">
+        <v>3500</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B6" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="38">
+        <f>SUM(C4:C5)</f>
+        <v>5500</v>
+      </c>
+      <c r="D6" s="38">
+        <f>SUM(D4:D5)</f>
+        <v>1750</v>
+      </c>
+      <c r="E6" s="38">
+        <f>SUM(E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="38">
+        <f>SUM(F4:F5)+O6</f>
+        <v>17250</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -3394,26 +3482,41 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="N6" s="38">
+        <f t="shared" ref="N6:P6" si="0">SUM(N4:N5)</f>
+        <v>2250</v>
+      </c>
+      <c r="O6" s="38">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="P6" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -3421,1462 +3524,1859 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>4000</v>
       </c>
-      <c r="D8">
-        <v>1000</v>
-      </c>
-      <c r="E8">
-        <v>1000</v>
-      </c>
       <c r="G8">
-        <f>SUM(C8:E8)</f>
         <v>6000</v>
       </c>
-      <c r="H8" s="10">
-        <f>D8/C8</f>
-        <v>0.25</v>
-      </c>
-      <c r="I8" s="2">
-        <f>C8*$C$1</f>
-        <v>400</v>
-      </c>
-      <c r="J8" s="2">
-        <f>D14-D8</f>
-        <v>100</v>
-      </c>
-      <c r="K8" s="2">
-        <f>I8+J8</f>
-        <v>500</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="2">
-        <f>D8</f>
-        <v>1000</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="3">
-        <f>E8/(C8+D8)</f>
-        <v>0.2</v>
-      </c>
-      <c r="U8">
-        <v>9000</v>
-      </c>
-      <c r="V8">
-        <v>14500</v>
-      </c>
-      <c r="W8" t="s">
-        <v>100</v>
-      </c>
-      <c r="X8">
+      <c r="H8">
+        <v>6000</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8">
+        <v>1500</v>
+      </c>
+      <c r="O8">
+        <v>250</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>9500</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1500</v>
-      </c>
-      <c r="D9">
+      <c r="G9">
+        <v>3000</v>
+      </c>
+      <c r="H9">
+        <v>3000</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9">
         <v>750</v>
       </c>
-      <c r="E9">
-        <v>750</v>
-      </c>
-      <c r="G9">
-        <f>SUM(C9:E9)</f>
-        <v>3000</v>
-      </c>
-      <c r="H9" s="10">
-        <f>D9/C9</f>
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="2">
-        <f>C11-I8</f>
-        <v>100</v>
-      </c>
-      <c r="J9" s="2">
-        <f>D15-D9</f>
-        <v>50</v>
-      </c>
-      <c r="K9" s="2">
-        <f>I9+J9</f>
-        <v>150</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="2">
-        <f>D9</f>
-        <v>750</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="3">
-        <f>E9/(C9+D9)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U9">
-        <v>3000</v>
-      </c>
-      <c r="V9">
-        <v>6250</v>
-      </c>
-      <c r="W9" t="s">
-        <v>101</v>
-      </c>
-      <c r="X9">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="O9">
+        <v>3500</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B10" s="38" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="38">
-        <f>SUM(C8:C9)</f>
-        <v>5500</v>
+        <f>SUM(C8:C9)+H8</f>
+        <v>6000</v>
       </c>
       <c r="D10" s="38">
-        <f t="shared" ref="D10:G10" si="0">SUM(D8:D9)</f>
-        <v>1750</v>
+        <f>SUM(D8:D9)+H9+N10</f>
+        <v>5250</v>
       </c>
       <c r="E10" s="38">
-        <f t="shared" si="0"/>
-        <v>1750</v>
-      </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38">
-        <f t="shared" si="0"/>
-        <v>9000</v>
-      </c>
-      <c r="H10" s="59">
-        <f>D10/C10</f>
-        <v>0.31818181818181818</v>
-      </c>
-      <c r="I10" s="60">
-        <f>SUM(I8:I9)</f>
-        <v>500</v>
-      </c>
-      <c r="J10" s="60">
-        <f>SUM(J8:J9)</f>
-        <v>150</v>
-      </c>
-      <c r="K10" s="61">
-        <f>I10+J10</f>
-        <v>650</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="2">
-        <f>D10</f>
-        <v>1750</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="3">
-        <f>E10/(C10+D10)</f>
-        <v>0.2413793103448276</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B11" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="43">
-        <f>G8-C10</f>
-        <v>500</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12">
-        <f>G9/G8</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
+        <f>SUM(E8:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="38">
+        <f>SUM(F8:F9)+O10</f>
+        <v>17250</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="38">
+        <f t="shared" ref="N10" si="1">SUM(N8:N9)</f>
+        <v>2250</v>
+      </c>
+      <c r="O10" s="38">
+        <f t="shared" ref="O10" si="2">SUM(O8:O9)</f>
+        <v>3750</v>
+      </c>
+      <c r="P10" s="38">
+        <f t="shared" ref="P10" si="3">SUM(P8:P9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
-        <f>C8+I8</f>
-        <v>4400</v>
-      </c>
-      <c r="D14" s="1">
-        <f>C14*H8</f>
-        <v>1100</v>
-      </c>
-      <c r="E14" s="1">
-        <f>D14</f>
-        <v>1100</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
+      <c r="C14">
+        <v>4000</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14">
+        <v>1000</v>
+      </c>
+      <c r="G14">
         <f>SUM(C14:E14)</f>
-        <v>6600</v>
-      </c>
-      <c r="H14" s="10">
+        <v>6000</v>
+      </c>
+      <c r="I14" s="10">
         <f>D14/C14</f>
         <v>0.25</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <f>C14*$C$1</f>
-        <v>440</v>
-      </c>
-      <c r="J14" s="2">
+        <v>400</v>
+      </c>
+      <c r="K14" s="2">
         <f>D20-D14</f>
-        <v>110</v>
-      </c>
-      <c r="K14" s="2">
-        <f>I14+J14</f>
-        <v>550</v>
+        <v>100</v>
       </c>
       <c r="L14" s="2">
-        <f>E8-K8</f>
+        <f>J14+K14</f>
         <v>500</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="2">
         <f>D14</f>
-        <v>1100</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="3">
         <f>E14/(C14+D14)</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="Z14">
+        <v>9000</v>
+      </c>
+      <c r="AA14">
+        <v>14500</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC14">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
-        <f>C9+C11-I8</f>
-        <v>1600</v>
-      </c>
-      <c r="D15" s="1">
-        <f>C15*H9</f>
-        <v>800</v>
-      </c>
-      <c r="E15" s="1">
-        <f>D15</f>
-        <v>800</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
+      <c r="C15">
+        <v>1500</v>
+      </c>
+      <c r="D15">
+        <v>750</v>
+      </c>
+      <c r="E15">
+        <v>750</v>
+      </c>
+      <c r="G15">
         <f>SUM(C15:E15)</f>
-        <v>3200</v>
-      </c>
-      <c r="H15" s="10">
+        <v>3000</v>
+      </c>
+      <c r="I15" s="10">
         <f>D15/C15</f>
         <v>0.5</v>
       </c>
-      <c r="I15" s="2">
-        <f>C17-I14</f>
-        <v>160</v>
-      </c>
       <c r="J15" s="2">
+        <f>C17-J14</f>
+        <v>100</v>
+      </c>
+      <c r="K15" s="2">
         <f>D21-D15</f>
-        <v>80</v>
-      </c>
-      <c r="K15" s="2">
-        <f>I15+J15</f>
-        <v>240</v>
+        <v>50</v>
       </c>
       <c r="L15" s="2">
-        <f>E9-K9</f>
-        <v>600</v>
-      </c>
-      <c r="M15" s="2">
+        <f>J15+K15</f>
+        <v>150</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="2">
         <f>D15</f>
-        <v>800</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="3">
+        <v>750</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="3">
         <f>E15/(C15+D15)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="P15" s="5">
-        <f>G14/G8</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B16" s="60" t="s">
+      <c r="Z15">
+        <v>3000</v>
+      </c>
+      <c r="AA15">
+        <v>6250</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC15">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="60">
+      <c r="C16" s="38">
         <f>SUM(C14:C15)</f>
-        <v>6000</v>
-      </c>
-      <c r="D16" s="60">
-        <f t="shared" ref="D16:G16" si="1">SUM(D14:D15)</f>
-        <v>1900</v>
-      </c>
-      <c r="E16" s="60">
-        <f t="shared" si="1"/>
-        <v>1900</v>
-      </c>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60">
-        <f t="shared" si="1"/>
-        <v>9800</v>
-      </c>
-      <c r="H16" s="59">
+        <v>5500</v>
+      </c>
+      <c r="D16" s="38">
+        <f t="shared" ref="D16:G16" si="4">SUM(D14:D15)</f>
+        <v>1750</v>
+      </c>
+      <c r="E16" s="38">
+        <f t="shared" si="4"/>
+        <v>1750</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38">
+        <f t="shared" si="4"/>
+        <v>9000</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="59">
         <f>D16/C16</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="I16" s="60">
-        <f>SUM(I14:I15)</f>
-        <v>600</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="J16" s="60">
-        <f t="shared" ref="J16" si="2">SUM(J14:J15)</f>
-        <v>190</v>
-      </c>
-      <c r="K16" s="61">
-        <f>I16+J16</f>
-        <v>790</v>
-      </c>
-      <c r="L16" s="2">
-        <f>E10-K10</f>
-        <v>1100</v>
-      </c>
-      <c r="M16" s="2">
+        <f>SUM(J14:J15)</f>
+        <v>500</v>
+      </c>
+      <c r="K16" s="60">
+        <f>SUM(K14:K15)</f>
+        <v>150</v>
+      </c>
+      <c r="L16" s="61">
+        <f>J16+K16</f>
+        <v>650</v>
+      </c>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="2">
         <f>D16</f>
-        <v>1900</v>
-      </c>
-      <c r="N16" s="2">
-        <f>L16+M16</f>
-        <v>3000</v>
-      </c>
-      <c r="O16" s="3">
+        <v>1750</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="3">
         <f>E16/(C16+D16)</f>
-        <v>0.24050632911392406</v>
-      </c>
-      <c r="P16" s="5">
-        <f>G15/G9</f>
-        <v>1.0666666666666667</v>
-      </c>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B17" s="62" t="s">
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B17" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="62">
+      <c r="C17" s="43">
         <f>G14-C16</f>
-        <v>600</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B18" s="43" t="s">
+        <v>500</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="64">
+      <c r="I18">
         <f>G15/G14</f>
-        <v>0.48484848484848486</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="64"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f>C14+I14</f>
-        <v>4840</v>
+        <f>C14+J14</f>
+        <v>4400</v>
       </c>
       <c r="D20" s="1">
-        <f>C20*H14</f>
-        <v>1210</v>
+        <f>C20*I14</f>
+        <v>1100</v>
       </c>
       <c r="E20" s="1">
         <f>D20</f>
-        <v>1210</v>
+        <v>1100</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1">
         <f>SUM(C20:E20)</f>
-        <v>7260</v>
-      </c>
-      <c r="H20" s="10">
+        <v>6600</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="10">
         <f>D20/C20</f>
         <v>0.25</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <f>C20*$C$1</f>
-        <v>484</v>
-      </c>
-      <c r="J20" s="2">
+        <v>440</v>
+      </c>
+      <c r="K20" s="2">
         <f>D26-D20</f>
-        <v>121</v>
-      </c>
-      <c r="K20" s="2">
-        <f>I20+J20</f>
-        <v>605</v>
+        <v>110</v>
       </c>
       <c r="L20" s="2">
-        <f>E14-K14</f>
+        <f>J20+K20</f>
         <v>550</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2">
+        <f>E14-L14</f>
+        <v>500</v>
+      </c>
+      <c r="R20" s="2">
         <f>D20</f>
-        <v>1210</v>
-      </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="3">
+        <v>1100</v>
+      </c>
+      <c r="S20" s="2"/>
+      <c r="T20" s="3">
         <f>E20/(C20+D20)</f>
         <v>0.2</v>
       </c>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <f>C15+C17-I14</f>
-        <v>1760</v>
+        <f>C15+C17-J14</f>
+        <v>1600</v>
       </c>
       <c r="D21" s="1">
-        <f>C21*H15</f>
-        <v>880</v>
+        <f>C21*I15</f>
+        <v>800</v>
       </c>
       <c r="E21" s="1">
         <f>D21</f>
-        <v>880</v>
+        <v>800</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
         <f>SUM(C21:E21)</f>
-        <v>3520</v>
-      </c>
-      <c r="H21" s="10">
+        <v>3200</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="10">
         <f>D21/C21</f>
         <v>0.5</v>
       </c>
-      <c r="I21" s="2">
-        <f>C23-I20</f>
-        <v>176</v>
-      </c>
       <c r="J21" s="2">
+        <f>C23-J20</f>
+        <v>160</v>
+      </c>
+      <c r="K21" s="2">
         <f>D27-D21</f>
-        <v>88</v>
-      </c>
-      <c r="K21" s="2">
-        <f>I21+J21</f>
-        <v>264</v>
+        <v>80</v>
       </c>
       <c r="L21" s="2">
-        <f>E15-K15</f>
-        <v>560</v>
-      </c>
-      <c r="M21" s="2">
+        <f>J21+K21</f>
+        <v>240</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2">
+        <f>E15-L15</f>
+        <v>600</v>
+      </c>
+      <c r="R21" s="2">
         <f>D21</f>
-        <v>880</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="3">
+        <v>800</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="T21" s="3">
         <f>E21/(C21+D21)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="P21" s="5">
+      <c r="U21" s="5">
         <f>G20/G14</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B22" s="60" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="60">
         <f>SUM(C20:C21)</f>
-        <v>6600</v>
+        <v>6000</v>
       </c>
       <c r="D22" s="60">
-        <f t="shared" ref="D22:G22" si="3">SUM(D20:D21)</f>
-        <v>2090</v>
+        <f t="shared" ref="D22:G22" si="5">SUM(D20:D21)</f>
+        <v>1900</v>
       </c>
       <c r="E22" s="60">
-        <f t="shared" si="3"/>
-        <v>2090</v>
+        <f t="shared" si="5"/>
+        <v>1900</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60">
-        <f t="shared" si="3"/>
-        <v>10780</v>
-      </c>
-      <c r="H22" s="59">
+        <f t="shared" si="5"/>
+        <v>9800</v>
+      </c>
+      <c r="H22" s="60"/>
+      <c r="I22" s="59">
         <f>D22/C22</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="I22" s="60">
-        <f>SUM(I20:I21)</f>
-        <v>660</v>
-      </c>
       <c r="J22" s="60">
-        <f t="shared" ref="J22" si="4">SUM(J20:J21)</f>
-        <v>209</v>
-      </c>
-      <c r="K22" s="61">
-        <f>I22+J22</f>
-        <v>869</v>
-      </c>
-      <c r="L22" s="2">
-        <f>E16-K16</f>
-        <v>1110</v>
-      </c>
-      <c r="M22" s="2">
+        <f>SUM(J20:J21)</f>
+        <v>600</v>
+      </c>
+      <c r="K22" s="60">
+        <f t="shared" ref="K22" si="6">SUM(K20:K21)</f>
+        <v>190</v>
+      </c>
+      <c r="L22" s="61">
+        <f>J22+K22</f>
+        <v>790</v>
+      </c>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="2">
+        <f>E16-L16</f>
+        <v>1100</v>
+      </c>
+      <c r="R22" s="2">
         <f>D22</f>
-        <v>2090</v>
-      </c>
-      <c r="N22" s="2">
-        <f>L22+M22</f>
-        <v>3200</v>
-      </c>
-      <c r="O22" s="3">
+        <v>1900</v>
+      </c>
+      <c r="S22" s="2">
+        <f>Q22+R22</f>
+        <v>3000</v>
+      </c>
+      <c r="T22" s="3">
         <f>E22/(C22+D22)</f>
         <v>0.24050632911392406</v>
       </c>
-      <c r="P22" s="5">
+      <c r="U22" s="5">
         <f>G21/G15</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B23" s="1" t="s">
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B23" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="62">
         <f>G20-C22</f>
-        <v>660</v>
+        <v>600</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B24" t="s">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B24" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="10">
+      <c r="C24" s="43"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="64">
         <f>G21/G20</f>
         <v>0.48484848484848486</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="64"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <f>C20+I20</f>
-        <v>5324</v>
+        <f>C20+J20</f>
+        <v>4840</v>
       </c>
       <c r="D26" s="1">
-        <f>C26*H20</f>
-        <v>1331</v>
+        <f>C26*I20</f>
+        <v>1210</v>
       </c>
       <c r="E26" s="1">
         <f>D26</f>
-        <v>1331</v>
+        <v>1210</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
         <f>SUM(C26:E26)</f>
-        <v>7986</v>
-      </c>
-      <c r="H26" s="10">
+        <v>7260</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="10">
         <f>D26/C26</f>
         <v>0.25</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <f>C26*$C$1</f>
-        <v>532.4</v>
-      </c>
-      <c r="J26" s="2">
-        <f>D31-D26</f>
-        <v>133.10000000000014</v>
+        <v>484</v>
       </c>
       <c r="K26" s="2">
-        <f>I26+J26</f>
-        <v>665.50000000000011</v>
+        <f>D32-D26</f>
+        <v>121</v>
       </c>
       <c r="L26" s="2">
-        <f>E20-K20</f>
+        <f>J26+K26</f>
         <v>605</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2">
+        <f>E20-L20</f>
+        <v>550</v>
+      </c>
+      <c r="R26" s="2">
         <f>D26</f>
-        <v>1331</v>
-      </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="3">
+        <v>1210</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="3">
         <f>E26/(C26+D26)</f>
         <v>0.2</v>
       </c>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1">
-        <f>C21+C23-I20</f>
-        <v>1936</v>
+        <f>C21+C23-J20</f>
+        <v>1760</v>
       </c>
       <c r="D27" s="1">
-        <f>C27*H21</f>
-        <v>968</v>
+        <f>C27*I21</f>
+        <v>880</v>
       </c>
       <c r="E27" s="1">
         <f>D27</f>
-        <v>968</v>
+        <v>880</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
         <f>SUM(C27:E27)</f>
-        <v>3872</v>
-      </c>
-      <c r="H27" s="10">
+        <v>3520</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="10">
         <f>D27/C27</f>
         <v>0.5</v>
       </c>
-      <c r="I27" s="2">
-        <f>C29-I26</f>
-        <v>193.60000000000002</v>
-      </c>
       <c r="J27" s="2">
-        <f>D32-D27</f>
-        <v>96.799999999999955</v>
+        <f>C29-J26</f>
+        <v>176</v>
       </c>
       <c r="K27" s="2">
-        <f>I27+J27</f>
-        <v>290.39999999999998</v>
+        <f>D33-D27</f>
+        <v>88</v>
       </c>
       <c r="L27" s="2">
-        <f>E21-K21</f>
-        <v>616</v>
-      </c>
-      <c r="M27" s="2">
+        <f>J27+K27</f>
+        <v>264</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2">
+        <f>E21-L21</f>
+        <v>560</v>
+      </c>
+      <c r="R27" s="2">
         <f>D27</f>
-        <v>968</v>
-      </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="3">
+        <v>880</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="3">
         <f>E27/(C27+D27)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="P27" s="5">
+      <c r="U27" s="5">
         <f>G26/G20</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B28" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="60">
         <f>SUM(C26:C27)</f>
-        <v>7260</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" ref="D28:G28" si="5">SUM(D26:D27)</f>
-        <v>2299</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="5"/>
-        <v>2299</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1">
-        <f t="shared" si="5"/>
-        <v>11858</v>
-      </c>
-      <c r="H28" s="10">
+        <v>6600</v>
+      </c>
+      <c r="D28" s="60">
+        <f t="shared" ref="D28:G28" si="7">SUM(D26:D27)</f>
+        <v>2090</v>
+      </c>
+      <c r="E28" s="60">
+        <f t="shared" si="7"/>
+        <v>2090</v>
+      </c>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60">
+        <f t="shared" si="7"/>
+        <v>10780</v>
+      </c>
+      <c r="H28" s="60"/>
+      <c r="I28" s="59">
         <f>D28/C28</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="I28" s="1">
-        <f>SUM(I26:I27)</f>
-        <v>726</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" ref="J28" si="6">SUM(J26:J27)</f>
-        <v>229.90000000000009</v>
-      </c>
-      <c r="K28" s="2">
-        <f>I28+J28</f>
-        <v>955.90000000000009</v>
-      </c>
-      <c r="L28" s="2">
-        <f>E22-K22</f>
-        <v>1221</v>
-      </c>
-      <c r="M28" s="2">
+      <c r="J28" s="60">
+        <f>SUM(J26:J27)</f>
+        <v>660</v>
+      </c>
+      <c r="K28" s="60">
+        <f t="shared" ref="K28" si="8">SUM(K26:K27)</f>
+        <v>209</v>
+      </c>
+      <c r="L28" s="61">
+        <f>J28+K28</f>
+        <v>869</v>
+      </c>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="2">
+        <f>E22-L22</f>
+        <v>1110</v>
+      </c>
+      <c r="R28" s="2">
         <f>D28</f>
-        <v>2299</v>
-      </c>
-      <c r="N28" s="2">
-        <f>L28+M28</f>
-        <v>3520</v>
-      </c>
-      <c r="O28" s="3">
+        <v>2090</v>
+      </c>
+      <c r="S28" s="2">
+        <f>Q28+R28</f>
+        <v>3200</v>
+      </c>
+      <c r="T28" s="3">
         <f>E28/(C28+D28)</f>
         <v>0.24050632911392406</v>
       </c>
-      <c r="P28" s="5">
+      <c r="U28" s="5">
         <f>G27/G21</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q28" s="58"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="1">
         <f>G26-C28</f>
-        <v>726</v>
+        <v>660</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" t="s">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I30" s="10">
         <f>G27/G26</f>
         <v>0.48484848484848486</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1">
-        <f>C26*1.1</f>
-        <v>5856.4000000000005</v>
-      </c>
-      <c r="D31" s="1">
-        <f>C31*H26</f>
-        <v>1464.1000000000001</v>
-      </c>
-      <c r="E31" s="1">
-        <f>D31</f>
-        <v>1464.1000000000001</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1">
-        <f>SUM(C31:E31)</f>
-        <v>8784.6</v>
-      </c>
-      <c r="H31" s="10">
-        <f>D31/C31</f>
-        <v>0.25</v>
-      </c>
-      <c r="I31" s="2">
-        <f>C31*$C$1</f>
-        <v>585.6400000000001</v>
-      </c>
-      <c r="J31" s="2">
-        <f>D36-D31</f>
-        <v>146.41000000000008</v>
-      </c>
-      <c r="K31" s="2">
-        <f>I31+J31</f>
-        <v>732.05000000000018</v>
-      </c>
-      <c r="L31" s="2">
-        <f>E26-K26</f>
-        <v>665.49999999999989</v>
-      </c>
-      <c r="M31" s="2">
-        <f>D31</f>
-        <v>1464.1000000000001</v>
-      </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="3">
-        <f>E31/(C31+D31)</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="P31" s="5"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
       <c r="C32" s="1">
-        <f>C27+C29-I26</f>
-        <v>2129.6</v>
+        <f>C26+J26</f>
+        <v>5324</v>
       </c>
       <c r="D32" s="1">
-        <f>C32*H27</f>
-        <v>1064.8</v>
+        <f>C32*I26</f>
+        <v>1331</v>
       </c>
       <c r="E32" s="1">
         <f>D32</f>
-        <v>1064.8</v>
+        <v>1331</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1">
         <f>SUM(C32:E32)</f>
-        <v>4259.2</v>
-      </c>
-      <c r="H32" s="10">
+        <v>7986</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="10">
         <f>D32/C32</f>
-        <v>0.5</v>
-      </c>
-      <c r="I32" s="2">
-        <f>C34-I31</f>
-        <v>212.96000000000026</v>
+        <v>0.25</v>
       </c>
       <c r="J32" s="2">
+        <f>C32*$C$1</f>
+        <v>532.4</v>
+      </c>
+      <c r="K32" s="2">
         <f>D37-D32</f>
-        <v>106.48000000000025</v>
-      </c>
-      <c r="K32" s="2">
-        <f>I32+J32</f>
-        <v>319.44000000000051</v>
+        <v>133.10000000000014</v>
       </c>
       <c r="L32" s="2">
-        <f>E27-K27</f>
-        <v>677.6</v>
-      </c>
-      <c r="M32" s="2">
+        <f>J32+K32</f>
+        <v>665.50000000000011</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2">
+        <f>E26-L26</f>
+        <v>605</v>
+      </c>
+      <c r="R32" s="2">
         <f>D32</f>
-        <v>1064.8</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" s="3">
+        <v>1331</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="3">
         <f>E32/(C32+D32)</f>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="P32" s="5">
-        <f>G31/G26</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>0.2</v>
+      </c>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>1</v>
       </c>
       <c r="C33" s="1">
-        <f>SUM(C31:C32)</f>
-        <v>7986</v>
+        <f>C27+C29-J26</f>
+        <v>1936</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" ref="D33:G33" si="7">SUM(D31:D32)</f>
-        <v>2528.9</v>
+        <f>C33*I27</f>
+        <v>968</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="7"/>
-        <v>2528.9</v>
+        <f>D33</f>
+        <v>968</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1">
-        <f t="shared" si="7"/>
-        <v>13043.8</v>
-      </c>
-      <c r="H33" s="10">
+        <f>SUM(C33:E33)</f>
+        <v>3872</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="10">
         <f>D33/C33</f>
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="2">
+        <f>C35-J32</f>
+        <v>193.60000000000002</v>
+      </c>
+      <c r="K33" s="2">
+        <f>D38-D33</f>
+        <v>96.799999999999955</v>
+      </c>
+      <c r="L33" s="2">
+        <f>J33+K33</f>
+        <v>290.39999999999998</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2">
+        <f>E27-L27</f>
+        <v>616</v>
+      </c>
+      <c r="R33" s="2">
+        <f>D33</f>
+        <v>968</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="3">
+        <f>E33/(C33+D33)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U33" s="5">
+        <f>G32/G26</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1">
+        <f>SUM(C32:C33)</f>
+        <v>7260</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" ref="D34:G34" si="9">SUM(D32:D33)</f>
+        <v>2299</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="9"/>
+        <v>2299</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
+        <f t="shared" si="9"/>
+        <v>11858</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="10">
+        <f>D34/C34</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="I33" s="1">
-        <f>SUM(I31:I32)</f>
-        <v>798.60000000000036</v>
-      </c>
-      <c r="J33" s="1">
-        <f t="shared" ref="J33" si="8">SUM(J31:J32)</f>
-        <v>252.89000000000033</v>
-      </c>
-      <c r="K33" s="2">
-        <f>I33+J33</f>
-        <v>1051.4900000000007</v>
-      </c>
-      <c r="L33" s="2">
-        <f>E28-K28</f>
-        <v>1343.1</v>
-      </c>
-      <c r="M33" s="2">
-        <f>D33</f>
-        <v>2528.9</v>
-      </c>
-      <c r="N33" s="2">
-        <f>L33+M33</f>
-        <v>3872</v>
-      </c>
-      <c r="O33" s="3">
-        <f>E33/(C33+D33)</f>
+      <c r="J34" s="1">
+        <f>SUM(J32:J33)</f>
+        <v>726</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" ref="K34" si="10">SUM(K32:K33)</f>
+        <v>229.90000000000009</v>
+      </c>
+      <c r="L34" s="2">
+        <f>J34+K34</f>
+        <v>955.90000000000009</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2">
+        <f>E28-L28</f>
+        <v>1221</v>
+      </c>
+      <c r="R34" s="2">
+        <f>D34</f>
+        <v>2299</v>
+      </c>
+      <c r="S34" s="2">
+        <f>Q34+R34</f>
+        <v>3520</v>
+      </c>
+      <c r="T34" s="3">
+        <f>E34/(C34+D34)</f>
         <v>0.24050632911392406</v>
       </c>
-      <c r="P33" s="5">
-        <f>G32/G27</f>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="Q33" s="57"/>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B34" s="1" t="s">
+      <c r="U34" s="5">
+        <f>G33/G27</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="V34" s="58"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="1">
-        <f>G31-C33</f>
-        <v>798.60000000000036</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" t="s">
+      <c r="C35" s="1">
+        <f>G32-C34</f>
+        <v>726</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="10">
-        <f>G32/G31</f>
-        <v>0.48484848484848481</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B36" t="s">
+      <c r="I35" s="10">
+        <f>G33/G32</f>
+        <v>0.48484848484848486</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="1">
-        <f>C31*1.1</f>
-        <v>6442.0400000000009</v>
-      </c>
-      <c r="D36" s="1">
-        <f>C36*H31</f>
-        <v>1610.5100000000002</v>
-      </c>
-      <c r="E36" s="1">
-        <f>D36</f>
-        <v>1610.5100000000002</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1">
-        <f>SUM(C36:E36)</f>
-        <v>9663.0600000000013</v>
-      </c>
-      <c r="H36" s="10">
-        <f>D36/C36</f>
-        <v>0.25</v>
-      </c>
-      <c r="I36" s="2">
-        <f>C36*$C$1</f>
-        <v>644.20400000000018</v>
-      </c>
-      <c r="J36" s="2">
-        <f>D41-D36</f>
-        <v>161.05100000000016</v>
-      </c>
-      <c r="K36" s="2">
-        <f>I36+J36</f>
-        <v>805.25500000000034</v>
-      </c>
-      <c r="L36" s="2">
-        <f>E31-K31</f>
-        <v>732.05</v>
-      </c>
-      <c r="M36" s="2">
-        <f>D36</f>
-        <v>1610.5100000000002</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="3">
-        <f>E36/(C36+D36)</f>
-        <v>0.2</v>
-      </c>
-      <c r="P36" s="5"/>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
       <c r="C37" s="1">
-        <f>C32+C34-I31</f>
-        <v>2342.5600000000004</v>
+        <f>C32*1.1</f>
+        <v>5856.4000000000005</v>
       </c>
       <c r="D37" s="1">
-        <f>C37*H32</f>
-        <v>1171.2800000000002</v>
+        <f>C37*I32</f>
+        <v>1464.1000000000001</v>
       </c>
       <c r="E37" s="1">
         <f>D37</f>
-        <v>1171.2800000000002</v>
+        <v>1464.1000000000001</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1">
         <f>SUM(C37:E37)</f>
-        <v>4685.1200000000008</v>
-      </c>
-      <c r="H37" s="10">
+        <v>8784.6</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="10">
         <f>D37/C37</f>
-        <v>0.5</v>
-      </c>
-      <c r="I37" s="2">
-        <f>C39-I36</f>
-        <v>234.25599999999895</v>
+        <v>0.25</v>
       </c>
       <c r="J37" s="2">
+        <f>C37*$C$1</f>
+        <v>585.6400000000001</v>
+      </c>
+      <c r="K37" s="2">
         <f>D42-D37</f>
-        <v>117.12799999999947</v>
-      </c>
-      <c r="K37" s="2">
-        <f>I37+J37</f>
-        <v>351.38399999999842</v>
+        <v>146.41000000000008</v>
       </c>
       <c r="L37" s="2">
-        <f>E32-K32</f>
-        <v>745.35999999999945</v>
-      </c>
-      <c r="M37" s="2">
+        <f>J37+K37</f>
+        <v>732.05000000000018</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2">
+        <f>E32-L32</f>
+        <v>665.49999999999989</v>
+      </c>
+      <c r="R37" s="2">
         <f>D37</f>
-        <v>1171.2800000000002</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" s="3">
+        <v>1464.1000000000001</v>
+      </c>
+      <c r="S37" s="2"/>
+      <c r="T37" s="3">
         <f>E37/(C37+D37)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P37" s="5">
-        <f>G36/G31</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="U37" s="5"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="1">
-        <f>SUM(C36:C37)</f>
-        <v>8784.6000000000022</v>
+        <f>C33+C35-J32</f>
+        <v>2129.6</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" ref="D38:G38" si="9">SUM(D36:D37)</f>
-        <v>2781.7900000000004</v>
+        <f>C38*I33</f>
+        <v>1064.8</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="9"/>
-        <v>2781.7900000000004</v>
+        <f>D38</f>
+        <v>1064.8</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1">
-        <f t="shared" si="9"/>
-        <v>14348.180000000002</v>
-      </c>
-      <c r="H38" s="10">
+        <f>SUM(C38:E38)</f>
+        <v>4259.2</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="10">
         <f>D38/C38</f>
+        <v>0.5</v>
+      </c>
+      <c r="J38" s="2">
+        <f>C40-J37</f>
+        <v>212.96000000000026</v>
+      </c>
+      <c r="K38" s="2">
+        <f>D43-D38</f>
+        <v>106.48000000000025</v>
+      </c>
+      <c r="L38" s="2">
+        <f>J38+K38</f>
+        <v>319.44000000000051</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2">
+        <f>E33-L33</f>
+        <v>677.6</v>
+      </c>
+      <c r="R38" s="2">
+        <f>D38</f>
+        <v>1064.8</v>
+      </c>
+      <c r="S38" s="2"/>
+      <c r="T38" s="3">
+        <f>E38/(C38+D38)</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="U38" s="5">
+        <f>G37/G32</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <f>SUM(C37:C38)</f>
+        <v>7986</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" ref="D39:G39" si="11">SUM(D37:D38)</f>
+        <v>2528.9</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="11"/>
+        <v>2528.9</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1">
+        <f t="shared" si="11"/>
+        <v>13043.8</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="10">
+        <f>D39/C39</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="I38" s="1">
-        <f>SUM(I36:I37)</f>
-        <v>878.45999999999913</v>
-      </c>
-      <c r="J38" s="1">
-        <f t="shared" ref="J38" si="10">SUM(J36:J37)</f>
-        <v>278.17899999999963</v>
-      </c>
-      <c r="K38" s="2">
-        <f>I38+J38</f>
-        <v>1156.6389999999988</v>
-      </c>
-      <c r="L38" s="2">
-        <f>E33-K33</f>
-        <v>1477.4099999999994</v>
-      </c>
-      <c r="M38" s="2">
-        <f>D38</f>
-        <v>2781.7900000000004</v>
-      </c>
-      <c r="N38" s="2">
-        <f>L38+M38</f>
-        <v>4259.2</v>
-      </c>
-      <c r="O38" s="3">
-        <f>E38/(C38+D38)</f>
-        <v>0.24050632911392403</v>
-      </c>
-      <c r="P38" s="5">
-        <f>G37/G32</f>
-        <v>1.1000000000000003</v>
-      </c>
-      <c r="Q38" s="57"/>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B39" s="1" t="s">
+      <c r="J39" s="1">
+        <f>SUM(J37:J38)</f>
+        <v>798.60000000000036</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" ref="K39" si="12">SUM(K37:K38)</f>
+        <v>252.89000000000033</v>
+      </c>
+      <c r="L39" s="2">
+        <f>J39+K39</f>
+        <v>1051.4900000000007</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2">
+        <f>E34-L34</f>
+        <v>1343.1</v>
+      </c>
+      <c r="R39" s="2">
+        <f>D39</f>
+        <v>2528.9</v>
+      </c>
+      <c r="S39" s="2">
+        <f>Q39+R39</f>
+        <v>3872</v>
+      </c>
+      <c r="T39" s="3">
+        <f>E39/(C39+D39)</f>
+        <v>0.24050632911392406</v>
+      </c>
+      <c r="U39" s="5">
+        <f>G38/G33</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="V39" s="57"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="1">
-        <f>G36-C38</f>
-        <v>878.45999999999913</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" t="s">
+      <c r="C40" s="1">
+        <f>G37-C39</f>
+        <v>798.60000000000036</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="10">
-        <f>G37/G36</f>
-        <v>0.48484848484848486</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="H40" s="10"/>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B41" t="s">
+      <c r="I40" s="10">
+        <f>G38/G37</f>
+        <v>0.48484848484848481</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B42" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="1">
-        <f>C36*1.1</f>
-        <v>7086.2440000000015</v>
-      </c>
-      <c r="D41" s="1">
-        <f>C41*H36</f>
-        <v>1771.5610000000004</v>
-      </c>
-      <c r="E41" s="1">
-        <f>D41</f>
-        <v>1771.5610000000004</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1">
-        <f>SUM(C41:E41)</f>
-        <v>10629.366000000002</v>
-      </c>
-      <c r="H41" s="10">
-        <f>D41/C41</f>
-        <v>0.25</v>
-      </c>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2">
-        <f>E36-K36</f>
-        <v>805.25499999999988</v>
-      </c>
-      <c r="M41" s="2">
-        <f>D41</f>
-        <v>1771.5610000000004</v>
-      </c>
-      <c r="N41" s="2"/>
-      <c r="P41" s="5"/>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
       <c r="C42" s="1">
-        <f>C37+C39-I36</f>
-        <v>2576.8159999999993</v>
+        <f>C37*1.1</f>
+        <v>6442.0400000000009</v>
       </c>
       <c r="D42" s="1">
-        <f>C42*H37</f>
-        <v>1288.4079999999997</v>
+        <f>C42*I37</f>
+        <v>1610.5100000000002</v>
       </c>
       <c r="E42" s="1">
         <f>D42</f>
-        <v>1288.4079999999997</v>
+        <v>1610.5100000000002</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1">
         <f>SUM(C42:E42)</f>
-        <v>5153.6319999999987</v>
-      </c>
-      <c r="H42" s="10">
+        <v>9663.0600000000013</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="10">
         <f>D42/C42</f>
-        <v>0.5</v>
-      </c>
-      <c r="K42" s="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J42" s="2">
+        <f>C42*$C$1</f>
+        <v>644.20400000000018</v>
+      </c>
+      <c r="K42" s="2">
+        <f>D47-D42</f>
+        <v>161.05100000000016</v>
+      </c>
       <c r="L42" s="2">
-        <f>E37-K37</f>
-        <v>819.89600000000178</v>
-      </c>
-      <c r="M42" s="2">
+        <f>J42+K42</f>
+        <v>805.25500000000034</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2">
+        <f>E37-L37</f>
+        <v>732.05</v>
+      </c>
+      <c r="R42" s="2">
         <f>D42</f>
-        <v>1288.4079999999997</v>
-      </c>
-      <c r="N42" s="2"/>
-      <c r="P42" s="5">
-        <f>G41/G36</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B43" s="1" t="s">
-        <v>7</v>
+        <v>1610.5100000000002</v>
+      </c>
+      <c r="S42" s="2"/>
+      <c r="T42" s="3">
+        <f>E42/(C42+D42)</f>
+        <v>0.2</v>
+      </c>
+      <c r="U42" s="5"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B43" t="s">
+        <v>1</v>
       </c>
       <c r="C43" s="1">
-        <f>SUM(C41:C42)</f>
-        <v>9663.0600000000013</v>
+        <f>C38+C40-J37</f>
+        <v>2342.5600000000004</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" ref="D43:G43" si="11">SUM(D41:D42)</f>
-        <v>3059.9690000000001</v>
+        <f>C43*I38</f>
+        <v>1171.2800000000002</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="11"/>
-        <v>3059.9690000000001</v>
+        <f>D43</f>
+        <v>1171.2800000000002</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1">
-        <f t="shared" si="11"/>
-        <v>15782.998</v>
-      </c>
-      <c r="H43" s="10">
+        <f>SUM(C43:E43)</f>
+        <v>4685.1200000000008</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="10">
         <f>D43/C43</f>
+        <v>0.5</v>
+      </c>
+      <c r="J43" s="2">
+        <f>C45-J42</f>
+        <v>234.25599999999895</v>
+      </c>
+      <c r="K43" s="2">
+        <f>D48-D43</f>
+        <v>117.12799999999947</v>
+      </c>
+      <c r="L43" s="2">
+        <f>J43+K43</f>
+        <v>351.38399999999842</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2">
+        <f>E38-L38</f>
+        <v>745.35999999999945</v>
+      </c>
+      <c r="R43" s="2">
+        <f>D43</f>
+        <v>1171.2800000000002</v>
+      </c>
+      <c r="S43" s="2"/>
+      <c r="T43" s="3">
+        <f>E43/(C43+D43)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U43" s="5">
+        <f>G42/G37</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1">
+        <f>SUM(C42:C43)</f>
+        <v>8784.6000000000022</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" ref="D44:G44" si="13">SUM(D42:D43)</f>
+        <v>2781.7900000000004</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="13"/>
+        <v>2781.7900000000004</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1">
+        <f t="shared" si="13"/>
+        <v>14348.180000000002</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="10">
+        <f>D44/C44</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2">
-        <f>E38-K38</f>
-        <v>1625.1510000000017</v>
-      </c>
-      <c r="M43" s="2">
-        <f>D43</f>
-        <v>3059.9690000000001</v>
-      </c>
-      <c r="N43" s="2">
-        <f>L43+M43</f>
-        <v>4685.1200000000017</v>
-      </c>
-      <c r="O43" s="3">
-        <f>E43/(C43+D43)</f>
-        <v>0.240506329113924</v>
-      </c>
-      <c r="P43" s="5">
-        <f>G42/G37</f>
-        <v>1.0999999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B44" s="1" t="s">
+      <c r="J44" s="1">
+        <f>SUM(J42:J43)</f>
+        <v>878.45999999999913</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" ref="K44" si="14">SUM(K42:K43)</f>
+        <v>278.17899999999963</v>
+      </c>
+      <c r="L44" s="2">
+        <f>J44+K44</f>
+        <v>1156.6389999999988</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2">
+        <f>E39-L39</f>
+        <v>1477.4099999999994</v>
+      </c>
+      <c r="R44" s="2">
+        <f>D44</f>
+        <v>2781.7900000000004</v>
+      </c>
+      <c r="S44" s="2">
+        <f>Q44+R44</f>
+        <v>4259.2</v>
+      </c>
+      <c r="T44" s="3">
+        <f>E44/(C44+D44)</f>
+        <v>0.24050632911392403</v>
+      </c>
+      <c r="U44" s="5">
+        <f>G43/G38</f>
+        <v>1.1000000000000003</v>
+      </c>
+      <c r="V44" s="57"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="1">
-        <f>G41-C43</f>
-        <v>966.30600000000049</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" t="s">
+      <c r="C45" s="1">
+        <f>G42-C44</f>
+        <v>878.45999999999913</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" t="s">
         <v>21</v>
       </c>
-      <c r="H44" s="10">
-        <f>G42/G41</f>
-        <v>0.48484848484848464</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="I45" s="10">
+        <f>G43/G42</f>
+        <v>0.48484848484848486</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <f>C42*1.1</f>
+        <v>7086.2440000000015</v>
+      </c>
+      <c r="D47" s="1">
+        <f>C47*I42</f>
+        <v>1771.5610000000004</v>
+      </c>
+      <c r="E47" s="1">
+        <f>D47</f>
+        <v>1771.5610000000004</v>
+      </c>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
+      <c r="G47" s="1">
+        <f>SUM(C47:E47)</f>
+        <v>10629.366000000002</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="10">
+        <f>D47/C47</f>
+        <v>0.25</v>
+      </c>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="P47" s="5"/>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2">
+        <f>E42-L42</f>
+        <v>805.25499999999988</v>
+      </c>
+      <c r="R47" s="2">
+        <f>D47</f>
+        <v>1771.5610000000004</v>
+      </c>
+      <c r="S47" s="2"/>
+      <c r="U47" s="5"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <f>C43+C45-J42</f>
+        <v>2576.8159999999993</v>
+      </c>
+      <c r="D48" s="1">
+        <f>C48*I43</f>
+        <v>1288.4079999999997</v>
+      </c>
+      <c r="E48" s="1">
+        <f>D48</f>
+        <v>1288.4079999999997</v>
+      </c>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="P48" s="5"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="G48" s="1">
+        <f>SUM(C48:E48)</f>
+        <v>5153.6319999999987</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="10">
+        <f>D48/C48</f>
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2">
+        <f>E43-L43</f>
+        <v>819.89600000000178</v>
+      </c>
+      <c r="R48" s="2">
+        <f>D48</f>
+        <v>1288.4079999999997</v>
+      </c>
+      <c r="S48" s="2"/>
+      <c r="U48" s="5">
+        <f>G47/G42</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1">
+        <f>SUM(C47:C48)</f>
+        <v>9663.0600000000013</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" ref="D49:G49" si="15">SUM(D47:D48)</f>
+        <v>3059.9690000000001</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="15"/>
+        <v>3059.9690000000001</v>
+      </c>
       <c r="F49" s="1"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="G49" s="1">
+        <f t="shared" si="15"/>
+        <v>15782.998</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="10">
+        <f>D49/C49</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2">
+        <f>E44-L44</f>
+        <v>1625.1510000000017</v>
+      </c>
+      <c r="R49" s="2">
+        <f>D49</f>
+        <v>3059.9690000000001</v>
+      </c>
+      <c r="S49" s="2">
+        <f>Q49+R49</f>
+        <v>4685.1200000000017</v>
+      </c>
+      <c r="T49" s="3">
+        <f>E49/(C49+D49)</f>
+        <v>0.240506329113924</v>
+      </c>
+      <c r="U49" s="5">
+        <f>G48/G43</f>
+        <v>1.0999999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1">
+        <f>G47-C49</f>
+        <v>966.30600000000049</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" s="10">
+        <f>G48/G47</f>
+        <v>0.48484848484848464</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="I52" s="2"/>
+      <c r="H52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
-      <c r="P52" s="5"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B53" s="1"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="P53" s="5"/>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="H53" s="1"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="U53" s="5"/>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="U54" s="5"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="I57" s="2"/>
+      <c r="H57" s="1"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
-      <c r="P57" s="5"/>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B58" s="1"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="P58" s="5"/>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="H58" s="1"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="U58" s="5"/>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="U59" s="5"/>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2"/>
+      <c r="S62" s="2"/>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+      <c r="S63" s="2"/>
+      <c r="U63" s="5"/>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="U64" s="5"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H10 H16" formula="1"/>
+    <ignoredError sqref="I16 I22" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
ER: DI and DII scales now set correctly but DI V, sales, etc are wrong
</commit_message>
<xml_diff>
--- a/supplementary/Expanded Reproduction/spreadsheet illustrations (for Moscow Plekhanov).xlsx
+++ b/supplementary/Expanded Reproduction/spreadsheet illustrations (for Moscow Plekhanov).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\My Works\REPOS\simulation-api\supplementary\Expanded Reproduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83310F19-F1AC-4EC2-BE3A-D95F3D29B1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87A2264-EBB0-429A-8646-18D32547E09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="110">
   <si>
     <t>DI</t>
   </si>
@@ -538,12 +538,18 @@
   <si>
     <t>Scale</t>
   </si>
+  <si>
+    <t>Trade after period 1</t>
+  </si>
+  <si>
+    <t>(RED = wrong or weird)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -552,8 +558,9 @@
     <numFmt numFmtId="168" formatCode="_-[$$-47C]* #,##0_-;\-[$$-47C]* #,##0_-;_-[$$-47C]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +630,12 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -771,7 +784,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -862,6 +875,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -888,9 +907,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1359,13 +1377,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>575734</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1412,13 +1430,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>55034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1465,13 +1483,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>529166</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>122767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1518,13 +1536,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>97367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>397933</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>122767</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1571,13 +1589,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>592666</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>55033</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>46567</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1621,13 +1639,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>67734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2557,10 +2575,10 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="65"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
@@ -2796,10 +2814,10 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="G12" s="65" t="s">
+      <c r="G12" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="65"/>
+      <c r="H12" s="67"/>
     </row>
     <row r="13" spans="1:16" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B13" s="6" t="s">
@@ -3208,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
-  <dimension ref="A1:AC65"/>
+  <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3219,7 +3237,7 @@
     <col min="1" max="1" width="9.61328125" customWidth="1"/>
     <col min="5" max="6" width="8.921875" customWidth="1"/>
     <col min="7" max="7" width="7.61328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.4609375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.07421875" customWidth="1"/>
     <col min="10" max="10" width="6.69140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.765625" bestFit="1" customWidth="1"/>
@@ -3247,12 +3265,15 @@
         <v>0.1</v>
       </c>
       <c r="T1"/>
-      <c r="V1" s="65" t="s">
+      <c r="V1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="W1" s="65"/>
+      <c r="W1" s="67"/>
     </row>
     <row r="2" spans="1:29" ht="83.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="66" t="s">
+        <v>109</v>
+      </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -3265,13 +3286,13 @@
       <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="65" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -3280,23 +3301,23 @@
       <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="74" t="s">
+      <c r="L2" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74" t="s">
+      <c r="M2" s="65"/>
+      <c r="N2" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="74" t="s">
+      <c r="O2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P2" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="Q2" s="74" t="s">
+      <c r="Q2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="74" t="s">
+      <c r="R2" s="65" t="s">
         <v>17</v>
       </c>
       <c r="S2" s="6" t="s">
@@ -3344,13 +3365,13 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
@@ -3568,13 +3589,13 @@
         <v>44</v>
       </c>
       <c r="N8">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>250</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -3617,13 +3638,13 @@
         <v>43</v>
       </c>
       <c r="N9">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>3500</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1750</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -3649,7 +3670,7 @@
       </c>
       <c r="D10" s="38">
         <f>SUM(D8:D9)+H9+N10</f>
-        <v>5250</v>
+        <v>3000</v>
       </c>
       <c r="E10" s="38">
         <f>SUM(E8:E9)</f>
@@ -3668,16 +3689,13 @@
       <c r="M10" s="6"/>
       <c r="N10" s="38">
         <f t="shared" ref="N10" si="1">SUM(N8:N9)</f>
-        <v>2250</v>
+        <v>0</v>
       </c>
       <c r="O10" s="38">
         <f t="shared" ref="O10" si="2">SUM(O8:O9)</f>
         <v>3750</v>
       </c>
-      <c r="P10" s="38">
-        <f t="shared" ref="P10" si="3">SUM(P8:P9)</f>
-        <v>0</v>
-      </c>
+      <c r="P10" s="38"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
@@ -3693,13 +3711,16 @@
       <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -3723,20 +3744,43 @@
       <c r="AC11" s="6"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="C12" s="77">
+        <v>4400</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2200</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>4800</v>
+      </c>
+      <c r="G12" s="7">
+        <v>6600</v>
+      </c>
+      <c r="H12" s="7">
+        <v>-6400</v>
+      </c>
+      <c r="I12" s="6">
+        <f>D12/C12</f>
+        <v>0.5</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="M12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7">
+        <v>-950</v>
+      </c>
+      <c r="P12">
+        <v>1500</v>
+      </c>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -3752,23 +3796,40 @@
       <c r="AC12" s="6"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="C13">
+        <v>1600</v>
+      </c>
+      <c r="D13">
+        <v>1600</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>9950</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>3000</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="M13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>3450</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -3784,1075 +3845,1076 @@
       <c r="AC13" s="6"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
+      <c r="B14" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="38">
+        <f>SUM(C12:C13)+H12</f>
+        <v>-400</v>
+      </c>
+      <c r="D14" s="38">
+        <f>SUM(D12:D13)+H13+N14</f>
+        <v>6800</v>
+      </c>
+      <c r="E14" s="38">
+        <f>SUM(E12:E13)</f>
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="F14" s="38">
+        <f>SUM(F12:F13)+O14</f>
+        <v>17250</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="38">
+        <f t="shared" ref="N14" si="3">SUM(N12:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="38">
+        <f t="shared" ref="O14" si="4">SUM(O12:O13)</f>
+        <v>2500</v>
+      </c>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>4000</v>
       </c>
-      <c r="D14">
+      <c r="D18">
         <v>1000</v>
       </c>
-      <c r="E14">
+      <c r="E18">
         <v>1000</v>
       </c>
-      <c r="G14">
-        <f>SUM(C14:E14)</f>
+      <c r="G18">
+        <f>SUM(C18:E18)</f>
         <v>6000</v>
       </c>
-      <c r="I14" s="10">
-        <f>D14/C14</f>
+      <c r="I18" s="10">
+        <f>D18/C18</f>
         <v>0.25</v>
       </c>
-      <c r="J14" s="2">
-        <f>C14*$C$1</f>
+      <c r="J18" s="2">
+        <f>C18*$C$1</f>
         <v>400</v>
       </c>
-      <c r="K14" s="2">
-        <f>D20-D14</f>
+      <c r="K18" s="2">
+        <f>D24-D18</f>
         <v>100</v>
       </c>
-      <c r="L14" s="2">
-        <f>J14+K14</f>
+      <c r="L18" s="2">
+        <f>J18+K18</f>
         <v>500</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="11" t="s">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="2">
-        <f>D14</f>
+      <c r="R18" s="2">
+        <f>D18</f>
         <v>1000</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="S18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="T14" s="3">
-        <f>E14/(C14+D14)</f>
+      <c r="T18" s="3">
+        <f>E18/(C18+D18)</f>
         <v>0.2</v>
       </c>
-      <c r="Z14">
+      <c r="Z18">
         <v>9000</v>
       </c>
-      <c r="AA14">
+      <c r="AA18">
         <v>14500</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB18" t="s">
         <v>100</v>
       </c>
-      <c r="AC14">
+      <c r="AC18">
         <v>9500</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C19">
         <v>1500</v>
       </c>
-      <c r="D15">
+      <c r="D19">
         <v>750</v>
       </c>
-      <c r="E15">
+      <c r="E19">
         <v>750</v>
       </c>
-      <c r="G15">
-        <f>SUM(C15:E15)</f>
+      <c r="G19">
+        <f>SUM(C19:E19)</f>
         <v>3000</v>
       </c>
-      <c r="I15" s="10">
-        <f>D15/C15</f>
+      <c r="I19" s="10">
+        <f>D19/C19</f>
         <v>0.5</v>
       </c>
-      <c r="J15" s="2">
-        <f>C17-J14</f>
+      <c r="J19" s="2">
+        <f>C21-J18</f>
         <v>100</v>
       </c>
-      <c r="K15" s="2">
-        <f>D21-D15</f>
+      <c r="K19" s="2">
+        <f>D25-D19</f>
         <v>50</v>
       </c>
-      <c r="L15" s="2">
-        <f>J15+K15</f>
+      <c r="L19" s="2">
+        <f>J19+K19</f>
         <v>150</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="11" t="s">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="2">
-        <f>D15</f>
+      <c r="R19" s="2">
+        <f>D19</f>
         <v>750</v>
       </c>
-      <c r="S15" s="11" t="s">
+      <c r="S19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="3">
-        <f>E15/(C15+D15)</f>
+      <c r="T19" s="3">
+        <f>E19/(C19+D19)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z15">
+      <c r="Z19">
         <v>3000</v>
       </c>
-      <c r="AA15">
+      <c r="AA19">
         <v>6250</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AB19" t="s">
         <v>101</v>
       </c>
-      <c r="AC15">
+      <c r="AC19">
         <v>4000</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="B16" s="38" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="38">
-        <f>SUM(C14:C15)</f>
+      <c r="C20" s="38">
+        <f>SUM(C18:C19)</f>
         <v>5500</v>
       </c>
-      <c r="D16" s="38">
-        <f t="shared" ref="D16:G16" si="4">SUM(D14:D15)</f>
+      <c r="D20" s="38">
+        <f t="shared" ref="D20:G20" si="5">SUM(D18:D19)</f>
         <v>1750</v>
       </c>
-      <c r="E16" s="38">
-        <f t="shared" si="4"/>
+      <c r="E20" s="38">
+        <f t="shared" si="5"/>
         <v>1750</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38">
-        <f t="shared" si="4"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38">
+        <f t="shared" si="5"/>
         <v>9000</v>
       </c>
-      <c r="H16" s="38"/>
-      <c r="I16" s="59">
-        <f>D16/C16</f>
+      <c r="H20" s="38"/>
+      <c r="I20" s="59">
+        <f>D20/C20</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="J16" s="60">
-        <f>SUM(J14:J15)</f>
+      <c r="J20" s="60">
+        <f>SUM(J18:J19)</f>
         <v>500</v>
       </c>
-      <c r="K16" s="60">
-        <f>SUM(K14:K15)</f>
+      <c r="K20" s="60">
+        <f>SUM(K18:K19)</f>
         <v>150</v>
       </c>
-      <c r="L16" s="61">
-        <f>J16+K16</f>
+      <c r="L20" s="61">
+        <f>J20+K20</f>
         <v>650</v>
       </c>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="11" t="s">
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="R16" s="2">
-        <f>D16</f>
-        <v>1750</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="T16" s="3">
-        <f>E16/(C16+D16)</f>
-        <v>0.2413793103448276</v>
-      </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B17" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="43">
-        <f>G14-C16</f>
-        <v>500</v>
-      </c>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18">
-        <f>G15/G14</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <f>C14+J14</f>
-        <v>4400</v>
-      </c>
-      <c r="D20" s="1">
-        <f>C20*I14</f>
-        <v>1100</v>
-      </c>
-      <c r="E20" s="1">
-        <f>D20</f>
-        <v>1100</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <f>SUM(C20:E20)</f>
-        <v>6600</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="10">
-        <f>D20/C20</f>
-        <v>0.25</v>
-      </c>
-      <c r="J20" s="2">
-        <f>C20*$C$1</f>
-        <v>440</v>
-      </c>
-      <c r="K20" s="2">
-        <f>D26-D20</f>
-        <v>110</v>
-      </c>
-      <c r="L20" s="2">
-        <f>J20+K20</f>
-        <v>550</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2">
-        <f>E14-L14</f>
-        <v>500</v>
       </c>
       <c r="R20" s="2">
         <f>D20</f>
-        <v>1100</v>
-      </c>
-      <c r="S20" s="2"/>
+        <v>1750</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="T20" s="3">
         <f>E20/(C20+D20)</f>
+        <v>0.2413793103448276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B21" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="43">
+        <f>G18-C20</f>
+        <v>500</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <f>G19/G18</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="C23" s="76">
+        <f>C25/C19</f>
+        <v>1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <f>C18+J18</f>
+        <v>4400</v>
+      </c>
+      <c r="D24" s="1">
+        <f>C24*I18</f>
+        <v>1100</v>
+      </c>
+      <c r="E24" s="1">
+        <f>D24</f>
+        <v>1100</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <f>SUM(C24:E24)</f>
+        <v>6600</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="10">
+        <f>D24/C24</f>
+        <v>0.25</v>
+      </c>
+      <c r="J24" s="2">
+        <f>C24*$C$1</f>
+        <v>440</v>
+      </c>
+      <c r="K24" s="2">
+        <f>D30-D24</f>
+        <v>110</v>
+      </c>
+      <c r="L24" s="2">
+        <f>J24+K24</f>
+        <v>550</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2">
+        <f>E18-L18</f>
+        <v>500</v>
+      </c>
+      <c r="R24" s="2">
+        <f>D24</f>
+        <v>1100</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="3">
+        <f>E24/(C24+D24)</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
-        <f>C15+C17-J14</f>
+      <c r="C25" s="1">
+        <f>C19+C21-J18</f>
         <v>1600</v>
       </c>
-      <c r="D21" s="1">
-        <f>C21*I15</f>
+      <c r="D25" s="1">
+        <f>C25*I19</f>
         <v>800</v>
       </c>
-      <c r="E21" s="1">
-        <f>D21</f>
+      <c r="E25" s="1">
+        <f>D25</f>
         <v>800</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1">
-        <f>SUM(C21:E21)</f>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <f>SUM(C25:E25)</f>
         <v>3200</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="10">
-        <f>D21/C21</f>
+      <c r="H25" s="1"/>
+      <c r="I25" s="10">
+        <f>D25/C25</f>
         <v>0.5</v>
       </c>
-      <c r="J21" s="2">
-        <f>C23-J20</f>
+      <c r="J25" s="2">
+        <f>C27-J24</f>
         <v>160</v>
       </c>
-      <c r="K21" s="2">
-        <f>D27-D21</f>
+      <c r="K25" s="2">
+        <f>D31-D25</f>
         <v>80</v>
       </c>
-      <c r="L21" s="2">
-        <f>J21+K21</f>
+      <c r="L25" s="2">
+        <f>J25+K25</f>
         <v>240</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2">
-        <f>E15-L15</f>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2">
+        <f>E19-L19</f>
         <v>600</v>
       </c>
-      <c r="R21" s="2">
-        <f>D21</f>
+      <c r="R25" s="2">
+        <f>D25</f>
         <v>800</v>
       </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="3">
-        <f>E21/(C21+D21)</f>
+      <c r="S25" s="2"/>
+      <c r="T25" s="3">
+        <f>E25/(C25+D25)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U21" s="5">
-        <f>G20/G14</f>
+      <c r="U25" s="5">
+        <f>G24/G18</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B22" s="60" t="s">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B26" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="60">
-        <f>SUM(C20:C21)</f>
+      <c r="C26" s="60">
+        <f>SUM(C24:C25)</f>
         <v>6000</v>
       </c>
-      <c r="D22" s="60">
-        <f t="shared" ref="D22:G22" si="5">SUM(D20:D21)</f>
+      <c r="D26" s="60">
+        <f t="shared" ref="D26:G26" si="6">SUM(D24:D25)</f>
         <v>1900</v>
       </c>
-      <c r="E22" s="60">
-        <f t="shared" si="5"/>
+      <c r="E26" s="60">
+        <f t="shared" si="6"/>
         <v>1900</v>
       </c>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60">
-        <f t="shared" si="5"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60">
+        <f t="shared" si="6"/>
         <v>9800</v>
       </c>
-      <c r="H22" s="60"/>
-      <c r="I22" s="59">
-        <f>D22/C22</f>
+      <c r="H26" s="60"/>
+      <c r="I26" s="59">
+        <f>D26/C26</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="J22" s="60">
-        <f>SUM(J20:J21)</f>
+      <c r="J26" s="60">
+        <f>SUM(J24:J25)</f>
         <v>600</v>
       </c>
-      <c r="K22" s="60">
-        <f t="shared" ref="K22" si="6">SUM(K20:K21)</f>
+      <c r="K26" s="60">
+        <f t="shared" ref="K26" si="7">SUM(K24:K25)</f>
         <v>190</v>
       </c>
-      <c r="L22" s="61">
-        <f>J22+K22</f>
+      <c r="L26" s="61">
+        <f>J26+K26</f>
         <v>790</v>
       </c>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="2">
-        <f>E16-L16</f>
-        <v>1100</v>
-      </c>
-      <c r="R22" s="2">
-        <f>D22</f>
-        <v>1900</v>
-      </c>
-      <c r="S22" s="2">
-        <f>Q22+R22</f>
-        <v>3000</v>
-      </c>
-      <c r="T22" s="3">
-        <f>E22/(C22+D22)</f>
-        <v>0.24050632911392406</v>
-      </c>
-      <c r="U22" s="5">
-        <f>G21/G15</f>
-        <v>1.0666666666666667</v>
-      </c>
-      <c r="X22" s="2"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B23" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="62">
-        <f>G20-C22</f>
-        <v>600</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B24" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="64">
-        <f>G21/G20</f>
-        <v>0.48484848484848486</v>
-      </c>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="64"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <f>C20+J20</f>
-        <v>4840</v>
-      </c>
-      <c r="D26" s="1">
-        <f>C26*I20</f>
-        <v>1210</v>
-      </c>
-      <c r="E26" s="1">
-        <f>D26</f>
-        <v>1210</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <f>SUM(C26:E26)</f>
-        <v>7260</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="10">
-        <f>D26/C26</f>
-        <v>0.25</v>
-      </c>
-      <c r="J26" s="2">
-        <f>C26*$C$1</f>
-        <v>484</v>
-      </c>
-      <c r="K26" s="2">
-        <f>D32-D26</f>
-        <v>121</v>
-      </c>
-      <c r="L26" s="2">
-        <f>J26+K26</f>
-        <v>605</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="61"/>
       <c r="Q26" s="2">
         <f>E20-L20</f>
-        <v>550</v>
+        <v>1100</v>
       </c>
       <c r="R26" s="2">
         <f>D26</f>
-        <v>1210</v>
-      </c>
-      <c r="S26" s="2"/>
+        <v>1900</v>
+      </c>
+      <c r="S26" s="2">
+        <f>Q26+R26</f>
+        <v>3000</v>
+      </c>
       <c r="T26" s="3">
         <f>E26/(C26+D26)</f>
+        <v>0.24050632911392406</v>
+      </c>
+      <c r="U26" s="5">
+        <f>G25/G19</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B27" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="62">
+        <f>G24-C26</f>
+        <v>600</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B28" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="64">
+        <f>G25/G24</f>
+        <v>0.48484848484848486</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="64"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <f>C24+J24</f>
+        <v>4840</v>
+      </c>
+      <c r="D30" s="1">
+        <f>C30*I24</f>
+        <v>1210</v>
+      </c>
+      <c r="E30" s="1">
+        <f>D30</f>
+        <v>1210</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
+        <f>SUM(C30:E30)</f>
+        <v>7260</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="10">
+        <f>D30/C30</f>
+        <v>0.25</v>
+      </c>
+      <c r="J30" s="2">
+        <f>C30*$C$1</f>
+        <v>484</v>
+      </c>
+      <c r="K30" s="2">
+        <f>D36-D30</f>
+        <v>121</v>
+      </c>
+      <c r="L30" s="2">
+        <f>J30+K30</f>
+        <v>605</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2">
+        <f>E24-L24</f>
+        <v>550</v>
+      </c>
+      <c r="R30" s="2">
+        <f>D30</f>
+        <v>1210</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="3">
+        <f>E30/(C30+D30)</f>
         <v>0.2</v>
       </c>
-      <c r="U26" s="5"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B27" t="s">
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <f>C21+C23-J20</f>
+      <c r="C31" s="1">
+        <f>C25+C27-J24</f>
         <v>1760</v>
       </c>
-      <c r="D27" s="1">
-        <f>C27*I21</f>
+      <c r="D31" s="1">
+        <f>C31*I25</f>
         <v>880</v>
       </c>
-      <c r="E27" s="1">
-        <f>D27</f>
+      <c r="E31" s="1">
+        <f>D31</f>
         <v>880</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1">
-        <f>SUM(C27:E27)</f>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
+        <f>SUM(C31:E31)</f>
         <v>3520</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="10">
-        <f>D27/C27</f>
+      <c r="H31" s="1"/>
+      <c r="I31" s="10">
+        <f>D31/C31</f>
         <v>0.5</v>
       </c>
-      <c r="J27" s="2">
-        <f>C29-J26</f>
+      <c r="J31" s="2">
+        <f>C33-J30</f>
         <v>176</v>
       </c>
-      <c r="K27" s="2">
-        <f>D33-D27</f>
+      <c r="K31" s="2">
+        <f>D37-D31</f>
         <v>88</v>
       </c>
-      <c r="L27" s="2">
-        <f>J27+K27</f>
+      <c r="L31" s="2">
+        <f>J31+K31</f>
         <v>264</v>
       </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2">
-        <f>E21-L21</f>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2">
+        <f>E25-L25</f>
         <v>560</v>
       </c>
-      <c r="R27" s="2">
-        <f>D27</f>
+      <c r="R31" s="2">
+        <f>D31</f>
         <v>880</v>
       </c>
-      <c r="S27" s="2"/>
-      <c r="T27" s="3">
-        <f>E27/(C27+D27)</f>
+      <c r="S31" s="2"/>
+      <c r="T31" s="3">
+        <f>E31/(C31+D31)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="U27" s="5">
-        <f>G26/G20</f>
+      <c r="U31" s="5">
+        <f>G30/G24</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B28" s="60" t="s">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="B32" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="60">
-        <f>SUM(C26:C27)</f>
+      <c r="C32" s="60">
+        <f>SUM(C30:C31)</f>
         <v>6600</v>
       </c>
-      <c r="D28" s="60">
-        <f t="shared" ref="D28:G28" si="7">SUM(D26:D27)</f>
+      <c r="D32" s="60">
+        <f t="shared" ref="D32:G32" si="8">SUM(D30:D31)</f>
         <v>2090</v>
       </c>
-      <c r="E28" s="60">
-        <f t="shared" si="7"/>
+      <c r="E32" s="60">
+        <f t="shared" si="8"/>
         <v>2090</v>
       </c>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60">
-        <f t="shared" si="7"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60">
+        <f t="shared" si="8"/>
         <v>10780</v>
       </c>
-      <c r="H28" s="60"/>
-      <c r="I28" s="59">
-        <f>D28/C28</f>
+      <c r="H32" s="60"/>
+      <c r="I32" s="59">
+        <f>D32/C32</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="J28" s="60">
-        <f>SUM(J26:J27)</f>
+      <c r="J32" s="60">
+        <f>SUM(J30:J31)</f>
         <v>660</v>
       </c>
-      <c r="K28" s="60">
-        <f t="shared" ref="K28" si="8">SUM(K26:K27)</f>
+      <c r="K32" s="60">
+        <f t="shared" ref="K32" si="9">SUM(K30:K31)</f>
         <v>209</v>
       </c>
-      <c r="L28" s="61">
-        <f>J28+K28</f>
+      <c r="L32" s="61">
+        <f>J32+K32</f>
         <v>869</v>
       </c>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="2">
-        <f>E22-L22</f>
-        <v>1110</v>
-      </c>
-      <c r="R28" s="2">
-        <f>D28</f>
-        <v>2090</v>
-      </c>
-      <c r="S28" s="2">
-        <f>Q28+R28</f>
-        <v>3200</v>
-      </c>
-      <c r="T28" s="3">
-        <f>E28/(C28+D28)</f>
-        <v>0.24050632911392406</v>
-      </c>
-      <c r="U28" s="5">
-        <f>G27/G21</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1">
-        <f>G26-C28</f>
-        <v>660</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="10">
-        <f>G27/G26</f>
-        <v>0.48484848484848486</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <f>C26+J26</f>
-        <v>5324</v>
-      </c>
-      <c r="D32" s="1">
-        <f>C32*I26</f>
-        <v>1331</v>
-      </c>
-      <c r="E32" s="1">
-        <f>D32</f>
-        <v>1331</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1">
-        <f>SUM(C32:E32)</f>
-        <v>7986</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="10">
-        <f>D32/C32</f>
-        <v>0.25</v>
-      </c>
-      <c r="J32" s="2">
-        <f>C32*$C$1</f>
-        <v>532.4</v>
-      </c>
-      <c r="K32" s="2">
-        <f>D37-D32</f>
-        <v>133.10000000000014</v>
-      </c>
-      <c r="L32" s="2">
-        <f>J32+K32</f>
-        <v>665.50000000000011</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
       <c r="Q32" s="2">
         <f>E26-L26</f>
-        <v>605</v>
+        <v>1110</v>
       </c>
       <c r="R32" s="2">
         <f>D32</f>
-        <v>1331</v>
-      </c>
-      <c r="S32" s="2"/>
+        <v>2090</v>
+      </c>
+      <c r="S32" s="2">
+        <f>Q32+R32</f>
+        <v>3200</v>
+      </c>
       <c r="T32" s="3">
         <f>E32/(C32+D32)</f>
+        <v>0.24050632911392406</v>
+      </c>
+      <c r="U32" s="5">
+        <f>G31/G25</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <f>G30-C32</f>
+        <v>660</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="10">
+        <f>G31/G30</f>
+        <v>0.48484848484848486</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="I35" s="10"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <f>C30+J30</f>
+        <v>5324</v>
+      </c>
+      <c r="D36" s="1">
+        <f>C36*I30</f>
+        <v>1331</v>
+      </c>
+      <c r="E36" s="1">
+        <f>D36</f>
+        <v>1331</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1">
+        <f>SUM(C36:E36)</f>
+        <v>7986</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="10">
+        <f>D36/C36</f>
+        <v>0.25</v>
+      </c>
+      <c r="J36" s="2">
+        <f>C36*$C$1</f>
+        <v>532.4</v>
+      </c>
+      <c r="K36" s="2">
+        <f>D41-D36</f>
+        <v>133.10000000000014</v>
+      </c>
+      <c r="L36" s="2">
+        <f>J36+K36</f>
+        <v>665.50000000000011</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2">
+        <f>E30-L30</f>
+        <v>605</v>
+      </c>
+      <c r="R36" s="2">
+        <f>D36</f>
+        <v>1331</v>
+      </c>
+      <c r="S36" s="2"/>
+      <c r="T36" s="3">
+        <f>E36/(C36+D36)</f>
         <v>0.2</v>
       </c>
-      <c r="U32" s="5"/>
-    </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1">
-        <f>C27+C29-J26</f>
-        <v>1936</v>
-      </c>
-      <c r="D33" s="1">
-        <f>C33*I27</f>
-        <v>968</v>
-      </c>
-      <c r="E33" s="1">
-        <f>D33</f>
-        <v>968</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1">
-        <f>SUM(C33:E33)</f>
-        <v>3872</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="10">
-        <f>D33/C33</f>
-        <v>0.5</v>
-      </c>
-      <c r="J33" s="2">
-        <f>C35-J32</f>
-        <v>193.60000000000002</v>
-      </c>
-      <c r="K33" s="2">
-        <f>D38-D33</f>
-        <v>96.799999999999955</v>
-      </c>
-      <c r="L33" s="2">
-        <f>J33+K33</f>
-        <v>290.39999999999998</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2">
-        <f>E27-L27</f>
-        <v>616</v>
-      </c>
-      <c r="R33" s="2">
-        <f>D33</f>
-        <v>968</v>
-      </c>
-      <c r="S33" s="2"/>
-      <c r="T33" s="3">
-        <f>E33/(C33+D33)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U33" s="5">
-        <f>G32/G26</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="1">
-        <f>SUM(C32:C33)</f>
-        <v>7260</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" ref="D34:G34" si="9">SUM(D32:D33)</f>
-        <v>2299</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="9"/>
-        <v>2299</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1">
-        <f t="shared" si="9"/>
-        <v>11858</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="10">
-        <f>D34/C34</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="J34" s="1">
-        <f>SUM(J32:J33)</f>
-        <v>726</v>
-      </c>
-      <c r="K34" s="1">
-        <f t="shared" ref="K34" si="10">SUM(K32:K33)</f>
-        <v>229.90000000000009</v>
-      </c>
-      <c r="L34" s="2">
-        <f>J34+K34</f>
-        <v>955.90000000000009</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2">
-        <f>E28-L28</f>
-        <v>1221</v>
-      </c>
-      <c r="R34" s="2">
-        <f>D34</f>
-        <v>2299</v>
-      </c>
-      <c r="S34" s="2">
-        <f>Q34+R34</f>
-        <v>3520</v>
-      </c>
-      <c r="T34" s="3">
-        <f>E34/(C34+D34)</f>
-        <v>0.24050632911392406</v>
-      </c>
-      <c r="U34" s="5">
-        <f>G33/G27</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="V34" s="58"/>
-    </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1">
-        <f>G32-C34</f>
-        <v>726</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35" s="10">
-        <f>G33/G32</f>
-        <v>0.48484848484848486</v>
-      </c>
-    </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="I36" s="10"/>
+      <c r="U36" s="5"/>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1">
-        <f>C32*1.1</f>
-        <v>5856.4000000000005</v>
+        <f>C31+C33-J30</f>
+        <v>1936</v>
       </c>
       <c r="D37" s="1">
-        <f>C37*I32</f>
-        <v>1464.1000000000001</v>
+        <f>C37*I31</f>
+        <v>968</v>
       </c>
       <c r="E37" s="1">
         <f>D37</f>
-        <v>1464.1000000000001</v>
+        <v>968</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1">
         <f>SUM(C37:E37)</f>
-        <v>8784.6</v>
+        <v>3872</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="10">
         <f>D37/C37</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J37" s="2">
-        <f>C37*$C$1</f>
-        <v>585.6400000000001</v>
+        <f>C39-J36</f>
+        <v>193.60000000000002</v>
       </c>
       <c r="K37" s="2">
         <f>D42-D37</f>
-        <v>146.41000000000008</v>
+        <v>96.799999999999955</v>
       </c>
       <c r="L37" s="2">
         <f>J37+K37</f>
-        <v>732.05000000000018</v>
+        <v>290.39999999999998</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2">
-        <f>E32-L32</f>
-        <v>665.49999999999989</v>
+        <f>E31-L31</f>
+        <v>616</v>
       </c>
       <c r="R37" s="2">
         <f>D37</f>
-        <v>1464.1000000000001</v>
+        <v>968</v>
       </c>
       <c r="S37" s="2"/>
       <c r="T37" s="3">
         <f>E37/(C37+D37)</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="U37" s="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U37" s="5">
+        <f>G36/G30</f>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B38" t="s">
-        <v>1</v>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C38" s="1">
-        <f>C33+C35-J32</f>
-        <v>2129.6</v>
+        <f>SUM(C36:C37)</f>
+        <v>7260</v>
       </c>
       <c r="D38" s="1">
-        <f>C38*I33</f>
-        <v>1064.8</v>
+        <f t="shared" ref="D38:G38" si="10">SUM(D36:D37)</f>
+        <v>2299</v>
       </c>
       <c r="E38" s="1">
-        <f>D38</f>
-        <v>1064.8</v>
+        <f t="shared" si="10"/>
+        <v>2299</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1">
-        <f>SUM(C38:E38)</f>
-        <v>4259.2</v>
+        <f t="shared" si="10"/>
+        <v>11858</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="10">
         <f>D38/C38</f>
-        <v>0.5</v>
-      </c>
-      <c r="J38" s="2">
-        <f>C40-J37</f>
-        <v>212.96000000000026</v>
-      </c>
-      <c r="K38" s="2">
-        <f>D43-D38</f>
-        <v>106.48000000000025</v>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="J38" s="1">
+        <f>SUM(J36:J37)</f>
+        <v>726</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" ref="K38" si="11">SUM(K36:K37)</f>
+        <v>229.90000000000009</v>
       </c>
       <c r="L38" s="2">
         <f>J38+K38</f>
-        <v>319.44000000000051</v>
+        <v>955.90000000000009</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2">
-        <f>E33-L33</f>
-        <v>677.6</v>
+        <f>E32-L32</f>
+        <v>1221</v>
       </c>
       <c r="R38" s="2">
         <f>D38</f>
-        <v>1064.8</v>
-      </c>
-      <c r="S38" s="2"/>
+        <v>2299</v>
+      </c>
+      <c r="S38" s="2">
+        <f>Q38+R38</f>
+        <v>3520</v>
+      </c>
       <c r="T38" s="3">
         <f>E38/(C38+D38)</f>
-        <v>0.33333333333333337</v>
+        <v>0.24050632911392406</v>
       </c>
       <c r="U38" s="5">
-        <f>G37/G32</f>
+        <f>G37/G31</f>
         <v>1.1000000000000001</v>
       </c>
+      <c r="V38" s="58"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C39" s="1">
-        <f>SUM(C37:C38)</f>
-        <v>7986</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" ref="D39:G39" si="11">SUM(D37:D38)</f>
-        <v>2528.9</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="11"/>
-        <v>2528.9</v>
-      </c>
+        <f>G36-C38</f>
+        <v>726</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1">
-        <f t="shared" si="11"/>
-        <v>13043.8</v>
-      </c>
-      <c r="H39" s="1"/>
+      <c r="G39" t="s">
+        <v>21</v>
+      </c>
       <c r="I39" s="10">
-        <f>D39/C39</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="J39" s="1">
-        <f>SUM(J37:J38)</f>
-        <v>798.60000000000036</v>
-      </c>
-      <c r="K39" s="1">
-        <f t="shared" ref="K39" si="12">SUM(K37:K38)</f>
-        <v>252.89000000000033</v>
-      </c>
-      <c r="L39" s="2">
-        <f>J39+K39</f>
-        <v>1051.4900000000007</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2">
-        <f>E34-L34</f>
-        <v>1343.1</v>
-      </c>
-      <c r="R39" s="2">
-        <f>D39</f>
-        <v>2528.9</v>
-      </c>
-      <c r="S39" s="2">
-        <f>Q39+R39</f>
-        <v>3872</v>
-      </c>
-      <c r="T39" s="3">
-        <f>E39/(C39+D39)</f>
-        <v>0.24050632911392406</v>
-      </c>
-      <c r="U39" s="5">
-        <f>G38/G33</f>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="V39" s="57"/>
+        <f>G37/G36</f>
+        <v>0.48484848484848486</v>
+      </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="1">
-        <f>G37-C39</f>
-        <v>798.60000000000036</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="10">
-        <f>G38/G37</f>
-        <v>0.48484848484848481</v>
-      </c>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="I41" s="10"/>
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <f>C36*1.1</f>
+        <v>5856.4000000000005</v>
+      </c>
+      <c r="D41" s="1">
+        <f>C41*I36</f>
+        <v>1464.1000000000001</v>
+      </c>
+      <c r="E41" s="1">
+        <f>D41</f>
+        <v>1464.1000000000001</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1">
+        <f>SUM(C41:E41)</f>
+        <v>8784.6</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="10">
+        <f>D41/C41</f>
+        <v>0.25</v>
+      </c>
+      <c r="J41" s="2">
+        <f>C41*$C$1</f>
+        <v>585.6400000000001</v>
+      </c>
+      <c r="K41" s="2">
+        <f>D46-D41</f>
+        <v>146.41000000000008</v>
+      </c>
+      <c r="L41" s="2">
+        <f>J41+K41</f>
+        <v>732.05000000000018</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2">
+        <f>E36-L36</f>
+        <v>665.49999999999989</v>
+      </c>
+      <c r="R41" s="2">
+        <f>D41</f>
+        <v>1464.1000000000001</v>
+      </c>
+      <c r="S41" s="2"/>
+      <c r="T41" s="3">
+        <f>E41/(C41+D41)</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="U41" s="5"/>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="1">
-        <f>C37*1.1</f>
-        <v>6442.0400000000009</v>
+        <f>C37+C39-J36</f>
+        <v>2129.6</v>
       </c>
       <c r="D42" s="1">
         <f>C42*I37</f>
-        <v>1610.5100000000002</v>
+        <v>1064.8</v>
       </c>
       <c r="E42" s="1">
         <f>D42</f>
-        <v>1610.5100000000002</v>
+        <v>1064.8</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1">
         <f>SUM(C42:E42)</f>
-        <v>9663.0600000000013</v>
+        <v>4259.2</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="10">
         <f>D42/C42</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J42" s="2">
-        <f>C42*$C$1</f>
-        <v>644.20400000000018</v>
+        <f>C44-J41</f>
+        <v>212.96000000000026</v>
       </c>
       <c r="K42" s="2">
         <f>D47-D42</f>
-        <v>161.05100000000016</v>
+        <v>106.48000000000025</v>
       </c>
       <c r="L42" s="2">
         <f>J42+K42</f>
-        <v>805.25500000000034</v>
+        <v>319.44000000000051</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -4860,56 +4922,59 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2">
         <f>E37-L37</f>
-        <v>732.05</v>
+        <v>677.6</v>
       </c>
       <c r="R42" s="2">
         <f>D42</f>
-        <v>1610.5100000000002</v>
+        <v>1064.8</v>
       </c>
       <c r="S42" s="2"/>
       <c r="T42" s="3">
         <f>E42/(C42+D42)</f>
-        <v>0.2</v>
-      </c>
-      <c r="U42" s="5"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="U42" s="5">
+        <f>G41/G36</f>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B43" t="s">
-        <v>1</v>
+      <c r="B43" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C43" s="1">
-        <f>C38+C40-J37</f>
-        <v>2342.5600000000004</v>
+        <f>SUM(C41:C42)</f>
+        <v>7986</v>
       </c>
       <c r="D43" s="1">
-        <f>C43*I38</f>
-        <v>1171.2800000000002</v>
+        <f t="shared" ref="D43:G43" si="12">SUM(D41:D42)</f>
+        <v>2528.9</v>
       </c>
       <c r="E43" s="1">
-        <f>D43</f>
-        <v>1171.2800000000002</v>
+        <f t="shared" si="12"/>
+        <v>2528.9</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1">
-        <f>SUM(C43:E43)</f>
-        <v>4685.1200000000008</v>
+        <f t="shared" si="12"/>
+        <v>13043.8</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="10">
         <f>D43/C43</f>
-        <v>0.5</v>
-      </c>
-      <c r="J43" s="2">
-        <f>C45-J42</f>
-        <v>234.25599999999895</v>
-      </c>
-      <c r="K43" s="2">
-        <f>D48-D43</f>
-        <v>117.12799999999947</v>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="J43" s="1">
+        <f>SUM(J41:J42)</f>
+        <v>798.60000000000036</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" ref="K43" si="13">SUM(K41:K42)</f>
+        <v>252.89000000000033</v>
       </c>
       <c r="L43" s="2">
         <f>J43+K43</f>
-        <v>351.38399999999842</v>
+        <v>1051.4900000000007</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -4917,329 +4982,426 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2">
         <f>E38-L38</f>
-        <v>745.35999999999945</v>
+        <v>1343.1</v>
       </c>
       <c r="R43" s="2">
         <f>D43</f>
-        <v>1171.2800000000002</v>
-      </c>
-      <c r="S43" s="2"/>
+        <v>2528.9</v>
+      </c>
+      <c r="S43" s="2">
+        <f>Q43+R43</f>
+        <v>3872</v>
+      </c>
       <c r="T43" s="3">
         <f>E43/(C43+D43)</f>
-        <v>0.33333333333333331</v>
+        <v>0.24050632911392406</v>
       </c>
       <c r="U43" s="5">
         <f>G42/G37</f>
-        <v>1.1000000000000001</v>
-      </c>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="V43" s="57"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C44" s="1">
-        <f>SUM(C42:C43)</f>
-        <v>8784.6000000000022</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" ref="D44:G44" si="13">SUM(D42:D43)</f>
-        <v>2781.7900000000004</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="13"/>
-        <v>2781.7900000000004</v>
-      </c>
+        <f>G41-C43</f>
+        <v>798.60000000000036</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1">
-        <f t="shared" si="13"/>
-        <v>14348.180000000002</v>
-      </c>
-      <c r="H44" s="1"/>
+      <c r="G44" t="s">
+        <v>21</v>
+      </c>
       <c r="I44" s="10">
-        <f>D44/C44</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="J44" s="1">
-        <f>SUM(J42:J43)</f>
-        <v>878.45999999999913</v>
-      </c>
-      <c r="K44" s="1">
-        <f t="shared" ref="K44" si="14">SUM(K42:K43)</f>
-        <v>278.17899999999963</v>
-      </c>
-      <c r="L44" s="2">
-        <f>J44+K44</f>
-        <v>1156.6389999999988</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2">
-        <f>E39-L39</f>
-        <v>1477.4099999999994</v>
-      </c>
-      <c r="R44" s="2">
-        <f>D44</f>
-        <v>2781.7900000000004</v>
-      </c>
-      <c r="S44" s="2">
-        <f>Q44+R44</f>
-        <v>4259.2</v>
-      </c>
-      <c r="T44" s="3">
-        <f>E44/(C44+D44)</f>
-        <v>0.24050632911392403</v>
-      </c>
-      <c r="U44" s="5">
-        <f>G43/G38</f>
-        <v>1.1000000000000003</v>
-      </c>
-      <c r="V44" s="57"/>
+        <f>G42/G41</f>
+        <v>0.48484848484848481</v>
+      </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="1">
-        <f>G42-C44</f>
-        <v>878.45999999999913</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="10">
-        <f>G43/G42</f>
-        <v>0.48484848484848486</v>
-      </c>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="I46" s="10"/>
+      <c r="B46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <f>C41*1.1</f>
+        <v>6442.0400000000009</v>
+      </c>
+      <c r="D46" s="1">
+        <f>C46*I41</f>
+        <v>1610.5100000000002</v>
+      </c>
+      <c r="E46" s="1">
+        <f>D46</f>
+        <v>1610.5100000000002</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1">
+        <f>SUM(C46:E46)</f>
+        <v>9663.0600000000013</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="10">
+        <f>D46/C46</f>
+        <v>0.25</v>
+      </c>
+      <c r="J46" s="2">
+        <f>C46*$C$1</f>
+        <v>644.20400000000018</v>
+      </c>
+      <c r="K46" s="2">
+        <f>D51-D46</f>
+        <v>161.05100000000016</v>
+      </c>
+      <c r="L46" s="2">
+        <f>J46+K46</f>
+        <v>805.25500000000034</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2">
+        <f>E41-L41</f>
+        <v>732.05</v>
+      </c>
+      <c r="R46" s="2">
+        <f>D46</f>
+        <v>1610.5100000000002</v>
+      </c>
+      <c r="S46" s="2"/>
+      <c r="T46" s="3">
+        <f>E46/(C46+D46)</f>
+        <v>0.2</v>
+      </c>
+      <c r="U46" s="5"/>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1">
-        <f>C42*1.1</f>
-        <v>7086.2440000000015</v>
+        <f>C42+C44-J41</f>
+        <v>2342.5600000000004</v>
       </c>
       <c r="D47" s="1">
         <f>C47*I42</f>
-        <v>1771.5610000000004</v>
+        <v>1171.2800000000002</v>
       </c>
       <c r="E47" s="1">
         <f>D47</f>
-        <v>1771.5610000000004</v>
+        <v>1171.2800000000002</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1">
         <f>SUM(C47:E47)</f>
-        <v>10629.366000000002</v>
+        <v>4685.1200000000008</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="10">
         <f>D47/C47</f>
-        <v>0.25</v>
-      </c>
-      <c r="L47" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="2">
+        <f>C49-J46</f>
+        <v>234.25599999999895</v>
+      </c>
+      <c r="K47" s="2">
+        <f>D52-D47</f>
+        <v>117.12799999999947</v>
+      </c>
+      <c r="L47" s="2">
+        <f>J47+K47</f>
+        <v>351.38399999999842</v>
+      </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2">
         <f>E42-L42</f>
-        <v>805.25499999999988</v>
+        <v>745.35999999999945</v>
       </c>
       <c r="R47" s="2">
         <f>D47</f>
-        <v>1771.5610000000004</v>
+        <v>1171.2800000000002</v>
       </c>
       <c r="S47" s="2"/>
-      <c r="U47" s="5"/>
+      <c r="T47" s="3">
+        <f>E47/(C47+D47)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U47" s="5">
+        <f>G46/G41</f>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B48" t="s">
-        <v>1</v>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C48" s="1">
-        <f>C43+C45-J42</f>
-        <v>2576.8159999999993</v>
+        <f>SUM(C46:C47)</f>
+        <v>8784.6000000000022</v>
       </c>
       <c r="D48" s="1">
-        <f>C48*I43</f>
-        <v>1288.4079999999997</v>
+        <f t="shared" ref="D48:G48" si="14">SUM(D46:D47)</f>
+        <v>2781.7900000000004</v>
       </c>
       <c r="E48" s="1">
-        <f>D48</f>
-        <v>1288.4079999999997</v>
+        <f t="shared" si="14"/>
+        <v>2781.7900000000004</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1">
-        <f>SUM(C48:E48)</f>
-        <v>5153.6319999999987</v>
+        <f t="shared" si="14"/>
+        <v>14348.180000000002</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="10">
         <f>D48/C48</f>
-        <v>0.5</v>
-      </c>
-      <c r="L48" s="2"/>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="J48" s="1">
+        <f>SUM(J46:J47)</f>
+        <v>878.45999999999913</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" ref="K48" si="15">SUM(K46:K47)</f>
+        <v>278.17899999999963</v>
+      </c>
+      <c r="L48" s="2">
+        <f>J48+K48</f>
+        <v>1156.6389999999988</v>
+      </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2">
         <f>E43-L43</f>
-        <v>819.89600000000178</v>
+        <v>1477.4099999999994</v>
       </c>
       <c r="R48" s="2">
         <f>D48</f>
-        <v>1288.4079999999997</v>
-      </c>
-      <c r="S48" s="2"/>
+        <v>2781.7900000000004</v>
+      </c>
+      <c r="S48" s="2">
+        <f>Q48+R48</f>
+        <v>4259.2</v>
+      </c>
+      <c r="T48" s="3">
+        <f>E48/(C48+D48)</f>
+        <v>0.24050632911392403</v>
+      </c>
       <c r="U48" s="5">
         <f>G47/G42</f>
-        <v>1.1000000000000001</v>
-      </c>
+        <v>1.1000000000000003</v>
+      </c>
+      <c r="V48" s="57"/>
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B49" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C49" s="1">
-        <f>SUM(C47:C48)</f>
-        <v>9663.0600000000013</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" ref="D49:G49" si="15">SUM(D47:D48)</f>
-        <v>3059.9690000000001</v>
-      </c>
-      <c r="E49" s="1">
-        <f t="shared" si="15"/>
-        <v>3059.9690000000001</v>
-      </c>
+        <f>G46-C48</f>
+        <v>878.45999999999913</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1">
-        <f t="shared" si="15"/>
-        <v>15782.998</v>
-      </c>
-      <c r="H49" s="1"/>
+      <c r="G49" t="s">
+        <v>21</v>
+      </c>
       <c r="I49" s="10">
-        <f>D49/C49</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2">
-        <f>E44-L44</f>
-        <v>1625.1510000000017</v>
-      </c>
-      <c r="R49" s="2">
-        <f>D49</f>
-        <v>3059.9690000000001</v>
-      </c>
-      <c r="S49" s="2">
-        <f>Q49+R49</f>
-        <v>4685.1200000000017</v>
-      </c>
-      <c r="T49" s="3">
-        <f>E49/(C49+D49)</f>
-        <v>0.240506329113924</v>
-      </c>
-      <c r="U49" s="5">
-        <f>G48/G43</f>
-        <v>1.0999999999999996</v>
+        <f>G47/G46</f>
+        <v>0.48484848484848486</v>
       </c>
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="B50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="1">
-        <f>G47-C49</f>
-        <v>966.30600000000049</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" t="s">
-        <v>21</v>
-      </c>
-      <c r="I50" s="10">
-        <f>G48/G47</f>
-        <v>0.48484848484848464</v>
-      </c>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <f>C46*1.1</f>
+        <v>7086.2440000000015</v>
+      </c>
+      <c r="D51" s="1">
+        <f>C51*I46</f>
+        <v>1771.5610000000004</v>
+      </c>
+      <c r="E51" s="1">
+        <f>D51</f>
+        <v>1771.5610000000004</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1">
+        <f>SUM(C51:E51)</f>
+        <v>10629.366000000002</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="10">
+        <f>D51/C51</f>
+        <v>0.25</v>
+      </c>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2">
+        <f>E46-L46</f>
+        <v>805.25499999999988</v>
+      </c>
+      <c r="R51" s="2">
+        <f>D51</f>
+        <v>1771.5610000000004</v>
+      </c>
+      <c r="S51" s="2"/>
+      <c r="U51" s="5"/>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <f>C47+C49-J46</f>
+        <v>2576.8159999999993</v>
+      </c>
+      <c r="D52" s="1">
+        <f>C52*I47</f>
+        <v>1288.4079999999997</v>
+      </c>
+      <c r="E52" s="1">
+        <f>D52</f>
+        <v>1288.4079999999997</v>
+      </c>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1">
+        <f>SUM(C52:E52)</f>
+        <v>5153.6319999999987</v>
+      </c>
       <c r="H52" s="1"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+      <c r="I52" s="10">
+        <f>D52/C52</f>
+        <v>0.5</v>
+      </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
+      <c r="Q52" s="2">
+        <f>E47-L47</f>
+        <v>819.89600000000178</v>
+      </c>
+      <c r="R52" s="2">
+        <f>D52</f>
+        <v>1288.4079999999997</v>
+      </c>
       <c r="S52" s="2"/>
+      <c r="U52" s="5">
+        <f>G51/G46</f>
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1">
+        <f>SUM(C51:C52)</f>
+        <v>9663.0600000000013</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" ref="D53:G53" si="16">SUM(D51:D52)</f>
+        <v>3059.9690000000001</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="16"/>
+        <v>3059.9690000000001</v>
+      </c>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="G53" s="1">
+        <f t="shared" si="16"/>
+        <v>15782.998</v>
+      </c>
       <c r="H53" s="1"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="I53" s="10">
+        <f>D53/C53</f>
+        <v>0.31666666666666665</v>
+      </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
-      <c r="U53" s="5"/>
+      <c r="Q53" s="2">
+        <f>E48-L48</f>
+        <v>1625.1510000000017</v>
+      </c>
+      <c r="R53" s="2">
+        <f>D53</f>
+        <v>3059.9690000000001</v>
+      </c>
+      <c r="S53" s="2">
+        <f>Q53+R53</f>
+        <v>4685.1200000000017</v>
+      </c>
+      <c r="T53" s="3">
+        <f>E53/(C53+D53)</f>
+        <v>0.240506329113924</v>
+      </c>
+      <c r="U53" s="5">
+        <f>G52/G47</f>
+        <v>1.0999999999999996</v>
+      </c>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1">
+        <f>G51-C53</f>
+        <v>966.30600000000049</v>
+      </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="U54" s="5"/>
-    </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="G54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" s="10">
+        <f>G52/G51</f>
+        <v>0.48484848484848464</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C57" s="1"/>
@@ -5258,24 +5420,26 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
+      <c r="U57" s="5"/>
     </row>
     <row r="58" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
-      <c r="S58" s="2"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
       <c r="U58" s="5"/>
     </row>
     <row r="59" spans="2:21" x14ac:dyDescent="0.4">
@@ -5284,26 +5448,24 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="U59" s="5"/>
-    </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.4">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+      <c r="S61" s="2"/>
     </row>
     <row r="62" spans="2:21" x14ac:dyDescent="0.4">
       <c r="C62" s="1"/>
@@ -5322,24 +5484,26 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
+      <c r="U62" s="5"/>
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
-      <c r="S63" s="2"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
       <c r="U63" s="5"/>
     </row>
     <row r="64" spans="2:21" x14ac:dyDescent="0.4">
@@ -5348,26 +5512,70 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="U64" s="5"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2"/>
+      <c r="S66" s="2"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2"/>
+      <c r="S67" s="2"/>
+      <c r="U67" s="5"/>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="U68" s="5"/>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5376,7 +5584,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I16 I22" formula="1"/>
+    <ignoredError sqref="I20 I26" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -6865,21 +7073,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="38" t="s">
@@ -6902,12 +7110,12 @@
       <c r="E3" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
@@ -6926,12 +7134,12 @@
         <f>B4+C4+D4</f>
         <v>375</v>
       </c>
-      <c r="H4" s="71" t="s">
+      <c r="H4" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -6950,12 +7158,12 @@
         <f>B5+C5+D5</f>
         <v>300</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
@@ -6974,12 +7182,12 @@
         <f>B6+C6+D6</f>
         <v>200</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="43" t="s">
@@ -7007,21 +7215,21 @@
       <c r="A9" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
-      <c r="H9" s="67" t="s">
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="H9" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="69"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:14" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B10" s="48" t="s">

</xml_diff>